<commit_message>
update p2.tex + preliminary planning
</commit_message>
<xml_diff>
--- a/Thesis Planning.xlsx
+++ b/Thesis Planning.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
   <si>
     <t>Plan</t>
   </si>
@@ -44,40 +44,7 @@
     <t>DURATION</t>
   </si>
   <si>
-    <t>PERIODS</t>
-  </si>
-  <si>
     <t>ACTIVITY</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <rFont val="Corbel"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Complete (beyond plan)</t>
-    </r>
   </si>
   <si>
     <t>P1 Presentation</t>
@@ -90,9 +57,6 @@
   </si>
   <si>
     <t>5 weeks</t>
-  </si>
-  <si>
-    <t>ID in a week</t>
   </si>
   <si>
     <t>Christmas Holidays</t>
@@ -120,9 +84,6 @@
   </si>
   <si>
     <t>1 week</t>
-  </si>
-  <si>
-    <t>Thesis Planner</t>
   </si>
   <si>
     <t>Converting topographic data to RDF</t>
@@ -154,6 +115,39 @@
   <si>
     <t>4 weeks</t>
   </si>
+  <si>
+    <t>Method to link data sets</t>
+  </si>
+  <si>
+    <t>Method to query data sets</t>
+  </si>
+  <si>
+    <t>Write thesis first draft</t>
+  </si>
+  <si>
+    <t>Improve thesis first draft</t>
+  </si>
+  <si>
+    <t>Other project</t>
+  </si>
+  <si>
+    <t>WEEKS</t>
+  </si>
+  <si>
+    <t>Collect data</t>
+  </si>
+  <si>
+    <t>13 weeks</t>
+  </si>
+  <si>
+    <t>Prepare P4 presentation</t>
+  </si>
+  <si>
+    <t>Prepare P5 presenation</t>
+  </si>
+  <si>
+    <t>Planning of the Thesis</t>
+  </si>
 </sst>
 </file>
 
@@ -162,7 +156,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\.m\.yy;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -241,8 +235,16 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="42"/>
+      <color theme="1"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -264,12 +266,6 @@
       <patternFill patternType="lightUp">
         <fgColor theme="7"/>
         <bgColor theme="9" tint="0.59996337778862885"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
@@ -343,11 +339,11 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -378,9 +374,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
@@ -408,7 +401,7 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -422,7 +415,1250 @@
     <cellStyle name="Period Highlight Control" xfId="7"/>
     <cellStyle name="Project Headers" xfId="4"/>
   </cellStyles>
-  <dxfs count="130">
+  <dxfs count="218">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2512,10 +3748,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:AM28"/>
+  <dimension ref="B2:AM33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -2523,7 +3759,7 @@
     <col min="1" max="1" width="2.625" customWidth="1"/>
     <col min="2" max="2" width="33.25" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.375" style="1" customWidth="1"/>
     <col min="5" max="5" width="4.25" style="1" customWidth="1"/>
     <col min="6" max="6" width="7" style="1" customWidth="1"/>
     <col min="7" max="7" width="7.125" style="1" customWidth="1"/>
@@ -2553,44 +3789,42 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:39" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
+      <c r="B2" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
     </row>
     <row r="3" spans="2:39" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
       <c r="F3" s="4"/>
-      <c r="AA3" s="13"/>
+      <c r="AA3" s="12"/>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1"/>
-      <c r="AH3" s="10"/>
-      <c r="AI3" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="6"/>
     </row>
     <row r="4" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
       <c r="H4" s="7"/>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="12" t="s">
         <v>0</v>
       </c>
       <c r="K4" s="8"/>
-      <c r="L4" s="13" t="s">
+      <c r="L4" s="12" t="s">
         <v>1</v>
       </c>
       <c r="N4" s="9"/>
-      <c r="O4" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="P4" s="13"/>
+      <c r="O4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="P4" s="12"/>
     </row>
     <row r="6" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
@@ -2602,7 +3836,7 @@
     </row>
     <row r="7" spans="2:39" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>2</v>
@@ -2612,7 +3846,7 @@
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -2621,118 +3855,118 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="14">
+      <c r="F8" s="13">
         <v>42317</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="13">
         <v>42324</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="13">
         <v>42331</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="13">
         <v>42338</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="13">
         <v>42345</v>
       </c>
-      <c r="K8" s="14">
+      <c r="K8" s="13">
         <v>42352</v>
       </c>
-      <c r="L8" s="14">
+      <c r="L8" s="13">
         <v>42359</v>
       </c>
-      <c r="M8" s="14">
+      <c r="M8" s="13">
         <v>42366</v>
       </c>
-      <c r="N8" s="14">
+      <c r="N8" s="13">
         <v>42373</v>
       </c>
-      <c r="O8" s="14">
+      <c r="O8" s="13">
         <v>42380</v>
       </c>
-      <c r="P8" s="14">
+      <c r="P8" s="13">
         <v>42387</v>
       </c>
-      <c r="Q8" s="14">
+      <c r="Q8" s="13">
         <v>42394</v>
       </c>
-      <c r="R8" s="14">
+      <c r="R8" s="13">
         <v>42401</v>
       </c>
-      <c r="S8" s="14">
+      <c r="S8" s="13">
         <v>42408</v>
       </c>
-      <c r="T8" s="14">
+      <c r="T8" s="13">
         <v>42415</v>
       </c>
-      <c r="U8" s="14">
+      <c r="U8" s="13">
         <v>42422</v>
       </c>
-      <c r="V8" s="14">
+      <c r="V8" s="13">
         <v>42429</v>
       </c>
-      <c r="W8" s="14">
+      <c r="W8" s="13">
         <v>42436</v>
       </c>
-      <c r="X8" s="14">
+      <c r="X8" s="13">
         <v>42443</v>
       </c>
-      <c r="Y8" s="14">
+      <c r="Y8" s="13">
         <v>42450</v>
       </c>
-      <c r="Z8" s="14">
+      <c r="Z8" s="13">
         <v>42457</v>
       </c>
-      <c r="AA8" s="14">
+      <c r="AA8" s="13">
         <v>42464</v>
       </c>
-      <c r="AB8" s="14">
+      <c r="AB8" s="13">
         <v>42471</v>
       </c>
-      <c r="AC8" s="14">
+      <c r="AC8" s="13">
         <v>42478</v>
       </c>
-      <c r="AD8" s="14">
+      <c r="AD8" s="13">
         <v>42485</v>
       </c>
-      <c r="AE8" s="14">
+      <c r="AE8" s="13">
         <v>42492</v>
       </c>
-      <c r="AF8" s="14">
+      <c r="AF8" s="13">
         <v>42499</v>
       </c>
-      <c r="AG8" s="14">
+      <c r="AG8" s="13">
         <v>42506</v>
       </c>
-      <c r="AH8" s="14">
+      <c r="AH8" s="13">
         <v>42513</v>
       </c>
-      <c r="AI8" s="14">
+      <c r="AI8" s="13">
         <v>42520</v>
       </c>
-      <c r="AJ8" s="14">
+      <c r="AJ8" s="13">
         <v>42527</v>
       </c>
-      <c r="AK8" s="14">
+      <c r="AK8" s="13">
         <v>42534</v>
       </c>
-      <c r="AL8" s="14">
+      <c r="AL8" s="13">
         <v>42541</v>
       </c>
-      <c r="AM8" s="14">
+      <c r="AM8" s="13">
         <v>42548</v>
       </c>
     </row>
     <row r="9" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="17">
+      <c r="B9" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="16">
         <v>42317</v>
       </c>
-      <c r="D9" s="16" t="s">
-        <v>10</v>
+      <c r="D9" s="15" t="s">
+        <v>8</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="9"/>
@@ -2742,16 +3976,15 @@
       <c r="K9" s="7"/>
     </row>
     <row r="10" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="17">
+      <c r="B10" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="16">
         <v>42338</v>
       </c>
-      <c r="D10" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="7"/>
+      <c r="D10" s="15" t="s">
+        <v>8</v>
+      </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
@@ -2760,343 +3993,736 @@
       <c r="N10" s="7"/>
     </row>
     <row r="11" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="17">
-        <v>42345</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
+      <c r="B11" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="16">
+        <v>42380</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="O11" s="17"/>
     </row>
     <row r="12" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="17">
-        <v>42380</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
+      <c r="B12" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="16">
+        <v>42317</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
     </row>
     <row r="13" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="16">
+        <v>42345</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C14" s="16">
         <v>42380</v>
       </c>
-      <c r="D13" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="O13" s="18"/>
+      <c r="D14" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
     </row>
-    <row r="14" spans="2:39" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="11"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="12"/>
-    </row>
-    <row r="15" spans="2:39" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="17">
-        <v>42318</v>
-      </c>
-      <c r="D15" s="16" t="s">
+    <row r="15" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="16">
+        <v>42401</v>
+      </c>
+      <c r="D15" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="8"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+      <c r="V15" s="7"/>
     </row>
     <row r="16" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="17">
-        <v>42379</v>
-      </c>
-      <c r="D16" s="16" t="s">
+      <c r="B16" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="16">
+        <v>42429</v>
+      </c>
+      <c r="D16" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="N16" s="7"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="7"/>
+      <c r="Y16" s="7"/>
+      <c r="Z16" s="7"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
     </row>
     <row r="17" spans="2:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="16">
+        <v>42394</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="7"/>
+      <c r="Z17" s="7"/>
+      <c r="AA17" s="7"/>
+      <c r="AB17" s="7"/>
+      <c r="AC17" s="7"/>
+      <c r="AD17" s="7"/>
+    </row>
+    <row r="18" spans="2:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="16">
+        <v>42492</v>
+      </c>
+      <c r="D18" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="17">
-        <v>42387</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="P17" s="7"/>
-    </row>
-    <row r="18" spans="2:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>8</v>
-      </c>
+      <c r="AE18" s="7"/>
     </row>
     <row r="19" spans="2:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="16">
+        <v>42499</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF19" s="7"/>
+      <c r="AG19" s="7"/>
+      <c r="AH19" s="7"/>
+      <c r="AI19" s="7"/>
+      <c r="AJ19" s="7"/>
+    </row>
+    <row r="20" spans="2:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="16">
+        <v>42534</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="AK20" s="7"/>
+    </row>
+    <row r="21" spans="2:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="10"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="11"/>
+    </row>
+    <row r="22" spans="2:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="16">
+        <v>42318</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" spans="2:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="16">
+        <v>42379</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="N23" s="7"/>
+    </row>
+    <row r="24" spans="2:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="16">
+        <v>42387</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="P24" s="7"/>
+    </row>
+    <row r="25" spans="2:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="2:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="16">
+        <v>42126</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD26" s="7"/>
+    </row>
+    <row r="27" spans="2:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="16">
+        <v>42133</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF27" s="7"/>
+    </row>
+    <row r="28" spans="2:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="17">
-        <v>42126</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD19" s="7"/>
+      <c r="C28" s="16">
+        <v>42168</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="AJ28" s="7"/>
     </row>
-    <row r="20" spans="2:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="17">
-        <v>42133</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF20" s="7"/>
+    <row r="29" spans="2:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="16">
+        <v>42175</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="AK29" t="s">
+        <v>26</v>
+      </c>
+      <c r="AL29" s="7"/>
     </row>
-    <row r="21" spans="2:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="17">
-        <v>42168</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="AJ21" s="7"/>
+    <row r="30" spans="2:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="10"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="11"/>
     </row>
-    <row r="22" spans="2:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="17">
-        <v>42175</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="AK22" t="s">
-        <v>30</v>
-      </c>
-      <c r="AL22" s="7"/>
+    <row r="31" spans="2:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="16">
+        <v>42325</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="7"/>
     </row>
-    <row r="23" spans="2:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="11"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="12"/>
+    <row r="32" spans="2:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="16">
+        <v>42361</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
     </row>
-    <row r="24" spans="2:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="17">
-        <v>42325</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="7"/>
-    </row>
-    <row r="25" spans="2:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="17">
-        <v>42361</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-    </row>
-    <row r="26" spans="2:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="15"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="16"/>
-    </row>
-    <row r="27" spans="2:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="15"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="16"/>
-    </row>
-    <row r="28" spans="2:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="11"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="12"/>
+    <row r="33" spans="2:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="14"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:D4"/>
   </mergeCells>
-  <conditionalFormatting sqref="G15:AM15 M9:AM9 F24 H24:O24 F25:K27 N25:AM27 O10:AM10 F28:AM28 T11:AM11 V12:AM12 P16:AM16 F16:H16 F17:O22 F13:N13 Q21:AI21 Q19:AC19 Q20:AE20 Q22:AK22 J26:Q27 Q17:AM18 P13:AM13 AF19:AM19 AG20:AM20 AM22 AL21:AM21 F14:AM14 Q23:AM24">
-    <cfRule type="expression" dxfId="129" priority="185">
+  <conditionalFormatting sqref="G22:AM22 F31 H31:O31 F32:K33 N32:AM33 O10:AM10 T13:AM13 V14:AM14 P23:AM23 F23:H23 F24:O29 Q28:AI28 Q26:AC26 Q27:AE27 Q29:AK29 J33:Q33 Q24:AM25 AF26:AM26 AG27:AM27 AM29 AL28:AM28 F21:AM21 Q30:AM31 P11:AM11 P19:AE19 AK19:AM19 P17 P15 P16:T16 Y15:AM15 AB16:AM16 AE17:AM17 M9:AM9 M12:AM12 F15:N17 F11:N11 F19:N19">
+    <cfRule type="expression" dxfId="217" priority="297">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="128" priority="187">
+    <cfRule type="expression" dxfId="216" priority="299">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="127" priority="188">
+    <cfRule type="expression" dxfId="215" priority="300">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="126" priority="189">
+    <cfRule type="expression" dxfId="214" priority="301">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="190">
+    <cfRule type="expression" dxfId="213" priority="302">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="191">
+    <cfRule type="expression" dxfId="212" priority="303">
       <formula>F$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="195">
+    <cfRule type="expression" dxfId="211" priority="307">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="196">
+    <cfRule type="expression" dxfId="210" priority="308">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29:AM29">
-    <cfRule type="expression" dxfId="121" priority="186">
+  <conditionalFormatting sqref="B34:AM34">
+    <cfRule type="expression" dxfId="209" priority="298">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8:AM8">
-    <cfRule type="expression" dxfId="120" priority="192">
+    <cfRule type="expression" dxfId="208" priority="304">
       <formula>F$8=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="expression" dxfId="119" priority="161">
+    <cfRule type="expression" dxfId="207" priority="273">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="162">
+    <cfRule type="expression" dxfId="206" priority="274">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="163">
+    <cfRule type="expression" dxfId="205" priority="275">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="164">
+    <cfRule type="expression" dxfId="204" priority="276">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="165">
+    <cfRule type="expression" dxfId="203" priority="277">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="166">
+    <cfRule type="expression" dxfId="202" priority="278">
       <formula>G$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="167">
+    <cfRule type="expression" dxfId="201" priority="279">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="168">
+    <cfRule type="expression" dxfId="200" priority="280">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="expression" dxfId="111" priority="153">
+    <cfRule type="expression" dxfId="199" priority="265">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="154">
+    <cfRule type="expression" dxfId="198" priority="266">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="155">
+    <cfRule type="expression" dxfId="197" priority="267">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="156">
+    <cfRule type="expression" dxfId="196" priority="268">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="157">
+    <cfRule type="expression" dxfId="195" priority="269">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="158">
+    <cfRule type="expression" dxfId="194" priority="270">
       <formula>F$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="159">
+    <cfRule type="expression" dxfId="193" priority="271">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="160">
+    <cfRule type="expression" dxfId="192" priority="272">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I16:M16">
-    <cfRule type="expression" dxfId="103" priority="113">
+  <conditionalFormatting sqref="I23:M23">
+    <cfRule type="expression" dxfId="191" priority="225">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="114">
+    <cfRule type="expression" dxfId="190" priority="226">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="115">
+    <cfRule type="expression" dxfId="189" priority="227">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="116">
+    <cfRule type="expression" dxfId="188" priority="228">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="117">
+    <cfRule type="expression" dxfId="187" priority="229">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="118">
+    <cfRule type="expression" dxfId="186" priority="230">
       <formula>I$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="119">
+    <cfRule type="expression" dxfId="185" priority="231">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="120">
+    <cfRule type="expression" dxfId="184" priority="232">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O16">
-    <cfRule type="expression" dxfId="95" priority="105">
+  <conditionalFormatting sqref="O23">
+    <cfRule type="expression" dxfId="183" priority="217">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="106">
+    <cfRule type="expression" dxfId="182" priority="218">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="107">
+    <cfRule type="expression" dxfId="181" priority="219">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="108">
+    <cfRule type="expression" dxfId="180" priority="220">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="109">
+    <cfRule type="expression" dxfId="179" priority="221">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="110">
+    <cfRule type="expression" dxfId="178" priority="222">
       <formula>O$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="111">
+    <cfRule type="expression" dxfId="177" priority="223">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="112">
+    <cfRule type="expression" dxfId="176" priority="224">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F12:J12 F11:I11">
+  <conditionalFormatting sqref="F14:J14 F13:I13">
+    <cfRule type="expression" dxfId="175" priority="201">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="174" priority="202">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="173" priority="203">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="172" priority="204">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="171" priority="205">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="170" priority="206">
+      <formula>F$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="169" priority="207">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="168" priority="208">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K14:N14">
+    <cfRule type="expression" dxfId="167" priority="193">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="166" priority="194">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="165" priority="195">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="164" priority="196">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="163" priority="197">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="162" priority="198">
+      <formula>K$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="161" priority="199">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="160" priority="200">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F30:O30">
+    <cfRule type="expression" dxfId="159" priority="177">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="158" priority="178">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="157" priority="179">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="156" priority="180">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="155" priority="181">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="154" priority="182">
+      <formula>F$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="153" priority="183">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="152" priority="184">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P25:P27">
+    <cfRule type="expression" dxfId="151" priority="169">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="150" priority="170">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="149" priority="171">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="148" priority="172">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="147" priority="173">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="146" priority="174">
+      <formula>P$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="145" priority="175">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="144" priority="176">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P28:P31">
+    <cfRule type="expression" dxfId="143" priority="161">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="142" priority="162">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="141" priority="163">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="140" priority="164">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="139" priority="165">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="138" priority="166">
+      <formula>P$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="137" priority="167">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="136" priority="168">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE26">
+    <cfRule type="expression" dxfId="135" priority="153">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="134" priority="154">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="133" priority="155">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="132" priority="156">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="131" priority="157">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="130" priority="158">
+      <formula>AE$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="129" priority="159">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="128" priority="160">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK28">
+    <cfRule type="expression" dxfId="127" priority="145">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="126" priority="146">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="125" priority="147">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="124" priority="148">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="123" priority="149">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="122" priority="150">
+      <formula>AK$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="121" priority="151">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="120" priority="152">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q13:S13">
+    <cfRule type="expression" dxfId="119" priority="137">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="118" priority="138">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="117" priority="139">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="116" priority="140">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="115" priority="141">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="114" priority="142">
+      <formula>Q$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="113" priority="143">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="112" priority="144">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T14:U14">
+    <cfRule type="expression" dxfId="111" priority="129">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="110" priority="130">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="109" priority="131">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="108" priority="132">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="107" priority="133">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="106" priority="134">
+      <formula>T$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="105" priority="135">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="104" priority="136">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L9">
+    <cfRule type="expression" dxfId="103" priority="121">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="102" priority="122">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="101" priority="123">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="100" priority="124">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="99" priority="125">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="98" priority="126">
+      <formula>L$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="97" priority="127">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="96" priority="128">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P13">
+    <cfRule type="expression" dxfId="95" priority="113">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="94" priority="114">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="93" priority="115">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="92" priority="116">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="91" priority="117">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="90" priority="118">
+      <formula>P$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="89" priority="119">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="88" priority="120">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O15:O17 O19">
     <cfRule type="expression" dxfId="87" priority="89">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -3113,7 +4739,7 @@
       <formula>Plan</formula>
     </cfRule>
     <cfRule type="expression" dxfId="82" priority="94">
-      <formula>F$8=period_selected</formula>
+      <formula>O$8=period_selected</formula>
     </cfRule>
     <cfRule type="expression" dxfId="81" priority="95">
       <formula>MOD(COLUMN(),2)</formula>
@@ -3122,189 +4748,189 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K12:N12">
-    <cfRule type="expression" dxfId="79" priority="81">
+  <conditionalFormatting sqref="S14">
+    <cfRule type="expression" dxfId="79" priority="49">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="82">
+    <cfRule type="expression" dxfId="78" priority="50">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="83">
+    <cfRule type="expression" dxfId="77" priority="51">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="84">
+    <cfRule type="expression" dxfId="76" priority="52">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="85">
+    <cfRule type="expression" dxfId="75" priority="53">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="86">
+    <cfRule type="expression" dxfId="74" priority="54">
+      <formula>S$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="73" priority="55">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="72" priority="56">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="expression" dxfId="71" priority="33">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="70" priority="34">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="69" priority="35">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="68" priority="36">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="67" priority="37">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="66" priority="38">
+      <formula>H$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="65" priority="39">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="40">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K12:L12">
+    <cfRule type="expression" dxfId="63" priority="25">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="62" priority="26">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="61" priority="27">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="60" priority="28">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="29">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="58" priority="30">
       <formula>K$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="87">
+    <cfRule type="expression" dxfId="57" priority="31">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="88">
+    <cfRule type="expression" dxfId="56" priority="32">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F23:O23">
-    <cfRule type="expression" dxfId="71" priority="65">
+  <conditionalFormatting sqref="X15">
+    <cfRule type="expression" dxfId="55" priority="81">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="66">
+    <cfRule type="expression" dxfId="54" priority="82">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="67">
+    <cfRule type="expression" dxfId="53" priority="83">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="68">
+    <cfRule type="expression" dxfId="52" priority="84">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="69">
+    <cfRule type="expression" dxfId="51" priority="85">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="70">
-      <formula>F$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="65" priority="71">
+    <cfRule type="expression" dxfId="50" priority="86">
+      <formula>X$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="87">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="72">
+    <cfRule type="expression" dxfId="48" priority="88">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P18:P20">
-    <cfRule type="expression" dxfId="63" priority="57">
+  <conditionalFormatting sqref="W15">
+    <cfRule type="expression" dxfId="47" priority="73">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="58">
+    <cfRule type="expression" dxfId="46" priority="74">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="59">
+    <cfRule type="expression" dxfId="45" priority="75">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="60">
+    <cfRule type="expression" dxfId="44" priority="76">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="61">
+    <cfRule type="expression" dxfId="43" priority="77">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="62">
-      <formula>P$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="57" priority="63">
+    <cfRule type="expression" dxfId="42" priority="78">
+      <formula>W$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="79">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="64">
+    <cfRule type="expression" dxfId="40" priority="80">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P21:P24">
-    <cfRule type="expression" dxfId="55" priority="49">
+  <conditionalFormatting sqref="U16">
+    <cfRule type="expression" dxfId="39" priority="65">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="50">
+    <cfRule type="expression" dxfId="38" priority="66">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="51">
+    <cfRule type="expression" dxfId="37" priority="67">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="52">
+    <cfRule type="expression" dxfId="36" priority="68">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="53">
+    <cfRule type="expression" dxfId="35" priority="69">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="54">
-      <formula>P$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="49" priority="55">
+    <cfRule type="expression" dxfId="34" priority="70">
+      <formula>U$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="71">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="56">
+    <cfRule type="expression" dxfId="32" priority="72">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE19">
-    <cfRule type="expression" dxfId="47" priority="41">
+  <conditionalFormatting sqref="Q15">
+    <cfRule type="expression" dxfId="31" priority="41">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="42">
+    <cfRule type="expression" dxfId="30" priority="42">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="43">
+    <cfRule type="expression" dxfId="29" priority="43">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="44">
+    <cfRule type="expression" dxfId="28" priority="44">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="45">
+    <cfRule type="expression" dxfId="27" priority="45">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="46">
-      <formula>AE$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="41" priority="47">
+    <cfRule type="expression" dxfId="26" priority="46">
+      <formula>Q$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="47">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="48">
+    <cfRule type="expression" dxfId="24" priority="48">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK21">
-    <cfRule type="expression" dxfId="39" priority="33">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="34">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="35">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="36">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="35" priority="37">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="34" priority="38">
-      <formula>AK$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="33" priority="39">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="40">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q11:S11">
-    <cfRule type="expression" dxfId="31" priority="25">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="30" priority="26">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="29" priority="27">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="28">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="29">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="30">
-      <formula>Q$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="31">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="32">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T12:U12">
+  <conditionalFormatting sqref="AA16">
     <cfRule type="expression" dxfId="23" priority="17">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -3321,7 +4947,7 @@
       <formula>Plan</formula>
     </cfRule>
     <cfRule type="expression" dxfId="18" priority="22">
-      <formula>T$8=period_selected</formula>
+      <formula>AA$8=period_selected</formula>
     </cfRule>
     <cfRule type="expression" dxfId="17" priority="23">
       <formula>MOD(COLUMN(),2)</formula>
@@ -3330,7 +4956,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L9">
+  <conditionalFormatting sqref="F18:AD18 AF18:AM18">
     <cfRule type="expression" dxfId="15" priority="9">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -3347,7 +4973,7 @@
       <formula>Plan</formula>
     </cfRule>
     <cfRule type="expression" dxfId="10" priority="14">
-      <formula>L$8=period_selected</formula>
+      <formula>F$8=period_selected</formula>
     </cfRule>
     <cfRule type="expression" dxfId="9" priority="15">
       <formula>MOD(COLUMN(),2)</formula>
@@ -3356,7 +4982,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P11">
+  <conditionalFormatting sqref="F20:AJ20 AL20:AM20">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -3373,7 +4999,7 @@
       <formula>Plan</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="6">
-      <formula>P$8=period_selected</formula>
+      <formula>F$8=period_selected</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="7">
       <formula>MOD(COLUMN(),2)</formula>

</xml_diff>

<commit_message>
added references and updated planning
</commit_message>
<xml_diff>
--- a/Thesis Planning.xlsx
+++ b/Thesis Planning.xlsx
@@ -146,7 +146,7 @@
     <t>Prepare P5 presenation</t>
   </si>
   <si>
-    <t>Planning of the Thesis</t>
+    <t>Thesis Planning</t>
   </si>
 </sst>
 </file>
@@ -3750,8 +3750,8 @@
   </sheetPr>
   <dimension ref="B2:AM33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -4272,7 +4272,7 @@
       <c r="D31" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G31" s="7"/>
+      <c r="G31" s="8"/>
     </row>
     <row r="32" spans="2:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="14" t="s">

</xml_diff>

<commit_message>
updated GANTT and tools and data chapter
</commit_message>
<xml_diff>
--- a/Thesis Planning.xlsx
+++ b/Thesis Planning.xlsx
@@ -3751,7 +3751,7 @@
   <dimension ref="B2:AM33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AW7" sqref="AW7"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -3764,9 +3764,9 @@
     <col min="6" max="6" width="7" style="1" customWidth="1"/>
     <col min="7" max="7" width="7.125" style="1" customWidth="1"/>
     <col min="8" max="8" width="7.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.75" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.75" style="1" customWidth="1"/>
     <col min="10" max="10" width="6.875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="6.75" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.25" style="1" customWidth="1"/>
     <col min="12" max="12" width="7.5" style="1" customWidth="1"/>
     <col min="13" max="13" width="7.375" style="1" customWidth="1"/>
     <col min="14" max="14" width="7.875" style="1" customWidth="1"/>
@@ -3971,7 +3971,7 @@
       <c r="F9" s="8"/>
       <c r="G9" s="9"/>
       <c r="H9" s="8"/>
-      <c r="I9" s="7"/>
+      <c r="I9" s="8"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
     </row>
@@ -3985,7 +3985,7 @@
       <c r="D10" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="7"/>
+      <c r="I10" s="8"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
       <c r="L10" s="9"/>
@@ -4017,7 +4017,7 @@
       <c r="F12" s="8"/>
       <c r="G12" s="9"/>
       <c r="H12" s="8"/>
-      <c r="I12" s="7"/>
+      <c r="I12" s="8"/>
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
final updates for first draft of P2 graduation proposal
</commit_message>
<xml_diff>
--- a/Thesis Planning.xlsx
+++ b/Thesis Planning.xlsx
@@ -3748,10 +3748,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:AM33"/>
+  <dimension ref="A2:AM33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:AN34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -3763,10 +3763,9 @@
     <col min="5" max="5" width="4.25" style="1" customWidth="1"/>
     <col min="6" max="6" width="7" style="1" customWidth="1"/>
     <col min="7" max="7" width="7.125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.75" style="1" customWidth="1"/>
+    <col min="8" max="9" width="7.5" style="1" customWidth="1"/>
     <col min="10" max="10" width="6.875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.25" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.125" style="1" customWidth="1"/>
     <col min="12" max="12" width="7.5" style="1" customWidth="1"/>
     <col min="13" max="13" width="7.375" style="1" customWidth="1"/>
     <col min="14" max="14" width="7.875" style="1" customWidth="1"/>
@@ -3788,14 +3787,14 @@
     <col min="37" max="39" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
         <v>38</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
     </row>
-    <row r="3" spans="2:39" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
@@ -3808,7 +3807,7 @@
       <c r="AH3" s="1"/>
       <c r="AI3" s="6"/>
     </row>
-    <row r="4" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
@@ -3826,7 +3825,7 @@
       </c>
       <c r="P4" s="12"/>
     </row>
-    <row r="6" spans="2:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -3834,7 +3833,7 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="2:39" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
@@ -3850,7 +3849,7 @@
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="2:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -3958,7 +3957,10 @@
         <v>42548</v>
       </c>
     </row>
-    <row r="9" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1</v>
+      </c>
       <c r="B9" s="14" t="s">
         <v>7</v>
       </c>
@@ -3973,9 +3975,12 @@
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
-      <c r="K9" s="7"/>
+      <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2</v>
+      </c>
       <c r="B10" s="14" t="s">
         <v>11</v>
       </c>
@@ -3987,12 +3992,15 @@
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
-      <c r="K10" s="7"/>
+      <c r="K10" s="8"/>
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
       <c r="N10" s="7"/>
     </row>
-    <row r="11" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>3</v>
+      </c>
       <c r="B11" s="14" t="s">
         <v>16</v>
       </c>
@@ -4004,7 +4012,10 @@
       </c>
       <c r="O11" s="17"/>
     </row>
-    <row r="12" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>4</v>
+      </c>
       <c r="B12" s="14" t="s">
         <v>34</v>
       </c>
@@ -4020,7 +4031,10 @@
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>5</v>
+      </c>
       <c r="B13" s="14" t="s">
         <v>18</v>
       </c>
@@ -4031,7 +4045,7 @@
         <v>27</v>
       </c>
       <c r="J13" s="8"/>
-      <c r="K13" s="7"/>
+      <c r="K13" s="8"/>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
       <c r="N13" s="7"/>
@@ -4039,7 +4053,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>6</v>
+      </c>
       <c r="B14" s="14" t="s">
         <v>19</v>
       </c>
@@ -4054,7 +4071,10 @@
       <c r="Q14" s="7"/>
       <c r="R14" s="7"/>
     </row>
-    <row r="15" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>7</v>
+      </c>
       <c r="B15" s="14" t="s">
         <v>28</v>
       </c>
@@ -4070,7 +4090,10 @@
       <c r="U15" s="7"/>
       <c r="V15" s="7"/>
     </row>
-    <row r="16" spans="2:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>8</v>
+      </c>
       <c r="B16" s="14" t="s">
         <v>29</v>
       </c>
@@ -4089,7 +4112,10 @@
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
     </row>
-    <row r="17" spans="2:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>9</v>
+      </c>
       <c r="B17" s="14" t="s">
         <v>30</v>
       </c>
@@ -4114,7 +4140,10 @@
       <c r="AC17" s="7"/>
       <c r="AD17" s="7"/>
     </row>
-    <row r="18" spans="2:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>10</v>
+      </c>
       <c r="B18" s="14" t="s">
         <v>36</v>
       </c>
@@ -4126,7 +4155,10 @@
       </c>
       <c r="AE18" s="7"/>
     </row>
-    <row r="19" spans="2:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>11</v>
+      </c>
       <c r="B19" s="14" t="s">
         <v>31</v>
       </c>
@@ -4142,7 +4174,10 @@
       <c r="AI19" s="7"/>
       <c r="AJ19" s="7"/>
     </row>
-    <row r="20" spans="2:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>12</v>
+      </c>
       <c r="B20" s="14" t="s">
         <v>37</v>
       </c>
@@ -4154,12 +4189,12 @@
       </c>
       <c r="AK20" s="7"/>
     </row>
-    <row r="21" spans="2:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="10"/>
       <c r="C21" s="16"/>
       <c r="D21" s="11"/>
     </row>
-    <row r="22" spans="2:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="14" t="s">
         <v>5</v>
       </c>
@@ -4171,7 +4206,7 @@
       </c>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="2:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="14" t="s">
         <v>15</v>
       </c>
@@ -4183,7 +4218,7 @@
       </c>
       <c r="N23" s="7"/>
     </row>
-    <row r="24" spans="2:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="14" t="s">
         <v>14</v>
       </c>
@@ -4195,7 +4230,7 @@
       </c>
       <c r="P24" s="7"/>
     </row>
-    <row r="25" spans="2:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="14" t="s">
         <v>21</v>
       </c>
@@ -4206,7 +4241,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="2:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="14" t="s">
         <v>20</v>
       </c>
@@ -4218,7 +4253,7 @@
       </c>
       <c r="AD26" s="7"/>
     </row>
-    <row r="27" spans="2:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="14" t="s">
         <v>23</v>
       </c>
@@ -4230,7 +4265,7 @@
       </c>
       <c r="AF27" s="7"/>
     </row>
-    <row r="28" spans="2:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="14" t="s">
         <v>24</v>
       </c>
@@ -4242,7 +4277,7 @@
       </c>
       <c r="AJ28" s="7"/>
     </row>
-    <row r="29" spans="2:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="14" t="s">
         <v>25</v>
       </c>
@@ -4257,12 +4292,12 @@
       </c>
       <c r="AL29" s="7"/>
     </row>
-    <row r="30" spans="2:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="10"/>
       <c r="C30" s="16"/>
       <c r="D30" s="11"/>
     </row>
-    <row r="31" spans="2:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="14" t="s">
         <v>32</v>
       </c>
@@ -4274,7 +4309,7 @@
       </c>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" spans="2:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="14" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
added updated planning figure
</commit_message>
<xml_diff>
--- a/Thesis Planning.xlsx
+++ b/Thesis Planning.xlsx
@@ -3995,7 +3995,7 @@
       <c r="K10" s="8"/>
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
-      <c r="N10" s="7"/>
+      <c r="N10" s="8"/>
     </row>
     <row r="11" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -4048,7 +4048,7 @@
       <c r="K13" s="8"/>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
-      <c r="N13" s="7"/>
+      <c r="N13" s="8"/>
       <c r="O13" s="7" t="s">
         <v>26</v>
       </c>
@@ -4319,8 +4319,8 @@
       <c r="D32" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="L32" s="7"/>
-      <c r="M32" s="7"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
     </row>
     <row r="33" spans="2:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="14"/>

</xml_diff>

<commit_message>
improving p2 document based on feedback
</commit_message>
<xml_diff>
--- a/Thesis Planning.xlsx
+++ b/Thesis Planning.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
   <si>
     <t>Plan</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>1 week</t>
-  </si>
-  <si>
-    <t>Converting topographic data to RDF</t>
   </si>
   <si>
     <t>Prepare sensor data sets</t>
@@ -147,6 +144,12 @@
   </si>
   <si>
     <t>Thesis Planning</t>
+  </si>
+  <si>
+    <t>Converting static data to RDF</t>
+  </si>
+  <si>
+    <t>2 weeks</t>
   </si>
 </sst>
 </file>
@@ -415,7 +418,572 @@
     <cellStyle name="Period Highlight Control" xfId="7"/>
     <cellStyle name="Project Headers" xfId="4"/>
   </cellStyles>
-  <dxfs count="218">
+  <dxfs count="258">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3750,8 +4318,8 @@
   </sheetPr>
   <dimension ref="A2:AM33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:AN34"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -3789,7 +4357,7 @@
   <sheetData>
     <row r="2" spans="1:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -3845,7 +4413,7 @@
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -4017,13 +4585,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="16">
         <v>42317</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="9"/>
@@ -4036,47 +4604,46 @@
         <v>5</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="C13" s="16">
         <v>42345</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
-      <c r="N13" s="8"/>
       <c r="O13" s="7" t="s">
-        <v>26</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="P13" s="7"/>
+      <c r="U13" s="7"/>
     </row>
     <row r="14" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>6</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="16">
         <v>42380</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
     </row>
     <row r="15" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>7</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="16">
         <v>42401</v>
@@ -4084,18 +4651,18 @@
       <c r="D15" s="15" t="s">
         <v>8</v>
       </c>
+      <c r="Q15" s="7"/>
       <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
       <c r="V15" s="7"/>
+      <c r="W15" s="7"/>
+      <c r="X15" s="7"/>
     </row>
     <row r="16" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>8</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="16">
         <v>42429</v>
@@ -4103,11 +4670,11 @@
       <c r="D16" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="V16" s="7"/>
-      <c r="W16" s="7"/>
-      <c r="X16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
       <c r="Y16" s="7"/>
       <c r="Z16" s="7"/>
+      <c r="AA16" s="7"/>
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
@@ -4117,13 +4684,13 @@
         <v>9</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="16">
         <v>42394</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q17" s="7"/>
       <c r="R17" s="7"/>
@@ -4145,7 +4712,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="16">
         <v>42492</v>
@@ -4160,7 +4727,7 @@
         <v>11</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="16">
         <v>42499</v>
@@ -4179,7 +4746,7 @@
         <v>12</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="16">
         <v>42534</v>
@@ -4216,7 +4783,7 @@
       <c r="D23" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="N23" s="7"/>
+      <c r="N23" s="8"/>
     </row>
     <row r="24" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="14" t="s">
@@ -4232,10 +4799,10 @@
     </row>
     <row r="25" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="18" t="s">
         <v>21</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>22</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>6</v>
@@ -4243,7 +4810,7 @@
     </row>
     <row r="26" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C26" s="16">
         <v>42126</v>
@@ -4255,7 +4822,7 @@
     </row>
     <row r="27" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C27" s="16">
         <v>42133</v>
@@ -4267,7 +4834,7 @@
     </row>
     <row r="28" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28" s="16">
         <v>42168</v>
@@ -4279,7 +4846,7 @@
     </row>
     <row r="29" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C29" s="16">
         <v>42175</v>
@@ -4288,7 +4855,7 @@
         <v>6</v>
       </c>
       <c r="AK29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AL29" s="7"/>
     </row>
@@ -4299,7 +4866,7 @@
     </row>
     <row r="31" spans="1:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C31" s="16">
         <v>42325</v>
@@ -4331,329 +4898,459 @@
   <mergeCells count="1">
     <mergeCell ref="B2:D4"/>
   </mergeCells>
-  <conditionalFormatting sqref="G22:AM22 F31 H31:O31 F32:K33 N32:AM33 O10:AM10 T13:AM13 V14:AM14 P23:AM23 F23:H23 F24:O29 Q28:AI28 Q26:AC26 Q27:AE27 Q29:AK29 J33:Q33 Q24:AM25 AF26:AM26 AG27:AM27 AM29 AL28:AM28 F21:AM21 Q30:AM31 P11:AM11 P19:AE19 AK19:AM19 P17 P15 P16:T16 Y15:AM15 AB16:AM16 AE17:AM17 M9:AM9 M12:AM12 F15:N17 F11:N11 F19:N19">
-    <cfRule type="expression" dxfId="217" priority="297">
+  <conditionalFormatting sqref="G22:AM22 F31 H31:O31 F32:K33 N32:AM33 O10:AM10 T13 P23:AM23 F23:H23 F24:O29 Q28:AI28 Q26:AC26 Q27:AE27 Q29:AK29 J33:Q33 Q24:AM25 AF26:AM26 AG27:AM27 AM29 AL28:AM28 F21:AM21 Q30:AM31 P11:AM11 P19:AE19 AK19:AM19 P17 P15 P16:R16 Y15:AM15 AB16:AM16 AE17:AM17 M9:AM9 M12:AM12 F15:N17 F11:N11 F19:N19 V13:AM14">
+    <cfRule type="expression" dxfId="257" priority="401">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="216" priority="299">
+    <cfRule type="expression" dxfId="256" priority="403">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="215" priority="300">
+    <cfRule type="expression" dxfId="255" priority="404">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="214" priority="301">
+    <cfRule type="expression" dxfId="254" priority="405">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="213" priority="302">
+    <cfRule type="expression" dxfId="253" priority="406">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="212" priority="303">
+    <cfRule type="expression" dxfId="252" priority="407">
       <formula>F$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="211" priority="307">
+    <cfRule type="expression" dxfId="251" priority="411">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="210" priority="308">
+    <cfRule type="expression" dxfId="250" priority="412">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34:AM34">
-    <cfRule type="expression" dxfId="209" priority="298">
+    <cfRule type="expression" dxfId="249" priority="402">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8:AM8">
-    <cfRule type="expression" dxfId="208" priority="304">
+    <cfRule type="expression" dxfId="248" priority="408">
       <formula>F$8=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="expression" dxfId="207" priority="273">
+    <cfRule type="expression" dxfId="247" priority="377">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="206" priority="274">
+    <cfRule type="expression" dxfId="246" priority="378">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="205" priority="275">
+    <cfRule type="expression" dxfId="245" priority="379">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="204" priority="276">
+    <cfRule type="expression" dxfId="244" priority="380">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="203" priority="277">
+    <cfRule type="expression" dxfId="243" priority="381">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="202" priority="278">
+    <cfRule type="expression" dxfId="242" priority="382">
       <formula>G$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="201" priority="279">
+    <cfRule type="expression" dxfId="241" priority="383">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="200" priority="280">
+    <cfRule type="expression" dxfId="240" priority="384">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="expression" dxfId="199" priority="265">
+    <cfRule type="expression" dxfId="239" priority="369">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="198" priority="266">
+    <cfRule type="expression" dxfId="238" priority="370">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="197" priority="267">
+    <cfRule type="expression" dxfId="237" priority="371">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="196" priority="268">
+    <cfRule type="expression" dxfId="236" priority="372">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="195" priority="269">
+    <cfRule type="expression" dxfId="235" priority="373">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="194" priority="270">
+    <cfRule type="expression" dxfId="234" priority="374">
       <formula>F$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="193" priority="271">
+    <cfRule type="expression" dxfId="233" priority="375">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="192" priority="272">
+    <cfRule type="expression" dxfId="232" priority="376">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23:M23">
-    <cfRule type="expression" dxfId="191" priority="225">
+    <cfRule type="expression" dxfId="231" priority="329">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="190" priority="226">
+    <cfRule type="expression" dxfId="230" priority="330">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="189" priority="227">
+    <cfRule type="expression" dxfId="229" priority="331">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="188" priority="228">
+    <cfRule type="expression" dxfId="228" priority="332">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="187" priority="229">
+    <cfRule type="expression" dxfId="227" priority="333">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="186" priority="230">
+    <cfRule type="expression" dxfId="226" priority="334">
       <formula>I$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="185" priority="231">
+    <cfRule type="expression" dxfId="225" priority="335">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="184" priority="232">
+    <cfRule type="expression" dxfId="224" priority="336">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O23">
-    <cfRule type="expression" dxfId="183" priority="217">
+    <cfRule type="expression" dxfId="223" priority="321">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="182" priority="218">
+    <cfRule type="expression" dxfId="222" priority="322">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="181" priority="219">
+    <cfRule type="expression" dxfId="221" priority="323">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="180" priority="220">
+    <cfRule type="expression" dxfId="220" priority="324">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="179" priority="221">
+    <cfRule type="expression" dxfId="219" priority="325">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="178" priority="222">
+    <cfRule type="expression" dxfId="218" priority="326">
       <formula>O$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="177" priority="223">
+    <cfRule type="expression" dxfId="217" priority="327">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="176" priority="224">
+    <cfRule type="expression" dxfId="216" priority="328">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14:J14 F13:I13">
-    <cfRule type="expression" dxfId="175" priority="201">
+    <cfRule type="expression" dxfId="215" priority="305">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="174" priority="202">
+    <cfRule type="expression" dxfId="214" priority="306">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="173" priority="203">
+    <cfRule type="expression" dxfId="213" priority="307">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="172" priority="204">
+    <cfRule type="expression" dxfId="212" priority="308">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="171" priority="205">
+    <cfRule type="expression" dxfId="211" priority="309">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="170" priority="206">
+    <cfRule type="expression" dxfId="210" priority="310">
       <formula>F$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="169" priority="207">
+    <cfRule type="expression" dxfId="209" priority="311">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="168" priority="208">
+    <cfRule type="expression" dxfId="208" priority="312">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14:N14">
-    <cfRule type="expression" dxfId="167" priority="193">
+    <cfRule type="expression" dxfId="207" priority="297">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="166" priority="194">
+    <cfRule type="expression" dxfId="206" priority="298">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="165" priority="195">
+    <cfRule type="expression" dxfId="205" priority="299">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="164" priority="196">
+    <cfRule type="expression" dxfId="204" priority="300">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="163" priority="197">
+    <cfRule type="expression" dxfId="203" priority="301">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="162" priority="198">
+    <cfRule type="expression" dxfId="202" priority="302">
       <formula>K$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="161" priority="199">
+    <cfRule type="expression" dxfId="201" priority="303">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="160" priority="200">
+    <cfRule type="expression" dxfId="200" priority="304">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30:O30">
-    <cfRule type="expression" dxfId="159" priority="177">
+    <cfRule type="expression" dxfId="199" priority="281">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="158" priority="178">
+    <cfRule type="expression" dxfId="198" priority="282">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="157" priority="179">
+    <cfRule type="expression" dxfId="197" priority="283">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="156" priority="180">
+    <cfRule type="expression" dxfId="196" priority="284">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="155" priority="181">
+    <cfRule type="expression" dxfId="195" priority="285">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="154" priority="182">
+    <cfRule type="expression" dxfId="194" priority="286">
       <formula>F$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="153" priority="183">
+    <cfRule type="expression" dxfId="193" priority="287">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="152" priority="184">
+    <cfRule type="expression" dxfId="192" priority="288">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P25:P27">
-    <cfRule type="expression" dxfId="151" priority="169">
+    <cfRule type="expression" dxfId="191" priority="273">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="150" priority="170">
+    <cfRule type="expression" dxfId="190" priority="274">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="149" priority="171">
+    <cfRule type="expression" dxfId="189" priority="275">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="148" priority="172">
+    <cfRule type="expression" dxfId="188" priority="276">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="147" priority="173">
+    <cfRule type="expression" dxfId="187" priority="277">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="146" priority="174">
+    <cfRule type="expression" dxfId="186" priority="278">
       <formula>P$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="145" priority="175">
+    <cfRule type="expression" dxfId="185" priority="279">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="144" priority="176">
+    <cfRule type="expression" dxfId="184" priority="280">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P28:P31">
-    <cfRule type="expression" dxfId="143" priority="161">
+    <cfRule type="expression" dxfId="183" priority="265">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="142" priority="162">
+    <cfRule type="expression" dxfId="182" priority="266">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="141" priority="163">
+    <cfRule type="expression" dxfId="181" priority="267">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="140" priority="164">
+    <cfRule type="expression" dxfId="180" priority="268">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="139" priority="165">
+    <cfRule type="expression" dxfId="179" priority="269">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="138" priority="166">
+    <cfRule type="expression" dxfId="178" priority="270">
       <formula>P$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="137" priority="167">
+    <cfRule type="expression" dxfId="177" priority="271">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="136" priority="168">
+    <cfRule type="expression" dxfId="176" priority="272">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE26">
-    <cfRule type="expression" dxfId="135" priority="153">
+    <cfRule type="expression" dxfId="175" priority="257">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="134" priority="154">
+    <cfRule type="expression" dxfId="174" priority="258">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="133" priority="155">
+    <cfRule type="expression" dxfId="173" priority="259">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="132" priority="156">
+    <cfRule type="expression" dxfId="172" priority="260">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="131" priority="157">
+    <cfRule type="expression" dxfId="171" priority="261">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="130" priority="158">
+    <cfRule type="expression" dxfId="170" priority="262">
       <formula>AE$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="129" priority="159">
+    <cfRule type="expression" dxfId="169" priority="263">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="128" priority="160">
+    <cfRule type="expression" dxfId="168" priority="264">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK28">
-    <cfRule type="expression" dxfId="127" priority="145">
+    <cfRule type="expression" dxfId="167" priority="249">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="126" priority="146">
+    <cfRule type="expression" dxfId="166" priority="250">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="147">
+    <cfRule type="expression" dxfId="165" priority="251">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="148">
+    <cfRule type="expression" dxfId="164" priority="252">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="149">
+    <cfRule type="expression" dxfId="163" priority="253">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="150">
+    <cfRule type="expression" dxfId="162" priority="254">
       <formula>AK$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="121" priority="151">
+    <cfRule type="expression" dxfId="161" priority="255">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="120" priority="152">
+    <cfRule type="expression" dxfId="160" priority="256">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q13:S13">
+    <cfRule type="expression" dxfId="159" priority="241">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="158" priority="242">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="157" priority="243">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="156" priority="244">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="155" priority="245">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="154" priority="246">
+      <formula>Q$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="153" priority="247">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="152" priority="248">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T14:U14">
+    <cfRule type="expression" dxfId="151" priority="233">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="150" priority="234">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="149" priority="235">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="148" priority="236">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="147" priority="237">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="146" priority="238">
+      <formula>T$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="145" priority="239">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="144" priority="240">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L9">
+    <cfRule type="expression" dxfId="143" priority="225">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="142" priority="226">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="141" priority="227">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="140" priority="228">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="139" priority="229">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="138" priority="230">
+      <formula>L$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="137" priority="231">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="136" priority="232">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O15:O17 O19">
+    <cfRule type="expression" dxfId="135" priority="193">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="134" priority="194">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="133" priority="195">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="132" priority="196">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="131" priority="197">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="130" priority="198">
+      <formula>O$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="129" priority="199">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="128" priority="200">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S14">
+    <cfRule type="expression" dxfId="127" priority="153">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="126" priority="154">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="125" priority="155">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="124" priority="156">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="123" priority="157">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="122" priority="158">
+      <formula>S$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="121" priority="159">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="120" priority="160">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
     <cfRule type="expression" dxfId="119" priority="137">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -4670,7 +5367,7 @@
       <formula>Plan</formula>
     </cfRule>
     <cfRule type="expression" dxfId="114" priority="142">
-      <formula>Q$8=period_selected</formula>
+      <formula>H$8=period_selected</formula>
     </cfRule>
     <cfRule type="expression" dxfId="113" priority="143">
       <formula>MOD(COLUMN(),2)</formula>
@@ -4679,7 +5376,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T14:U14">
+  <conditionalFormatting sqref="K12:L12">
     <cfRule type="expression" dxfId="111" priority="129">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -4696,7 +5393,7 @@
       <formula>Plan</formula>
     </cfRule>
     <cfRule type="expression" dxfId="106" priority="134">
-      <formula>T$8=period_selected</formula>
+      <formula>K$8=period_selected</formula>
     </cfRule>
     <cfRule type="expression" dxfId="105" priority="135">
       <formula>MOD(COLUMN(),2)</formula>
@@ -4705,33 +5402,33 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L9">
-    <cfRule type="expression" dxfId="103" priority="121">
+  <conditionalFormatting sqref="U16">
+    <cfRule type="expression" dxfId="103" priority="169">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="122">
+    <cfRule type="expression" dxfId="102" priority="170">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="123">
+    <cfRule type="expression" dxfId="101" priority="171">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="124">
+    <cfRule type="expression" dxfId="100" priority="172">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="125">
+    <cfRule type="expression" dxfId="99" priority="173">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="126">
-      <formula>L$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="97" priority="127">
+    <cfRule type="expression" dxfId="98" priority="174">
+      <formula>U$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="97" priority="175">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="128">
+    <cfRule type="expression" dxfId="96" priority="176">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P13">
+  <conditionalFormatting sqref="F18:AD18 AF18:AM18">
     <cfRule type="expression" dxfId="95" priority="113">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -4748,7 +5445,7 @@
       <formula>Plan</formula>
     </cfRule>
     <cfRule type="expression" dxfId="90" priority="118">
-      <formula>P$8=period_selected</formula>
+      <formula>F$8=period_selected</formula>
     </cfRule>
     <cfRule type="expression" dxfId="89" priority="119">
       <formula>MOD(COLUMN(),2)</formula>
@@ -4757,211 +5454,211 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O15:O17 O19">
-    <cfRule type="expression" dxfId="87" priority="89">
+  <conditionalFormatting sqref="F20:AJ20 AL20:AM20">
+    <cfRule type="expression" dxfId="87" priority="105">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="90">
+    <cfRule type="expression" dxfId="86" priority="106">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="91">
+    <cfRule type="expression" dxfId="85" priority="107">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="92">
+    <cfRule type="expression" dxfId="84" priority="108">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="93">
+    <cfRule type="expression" dxfId="83" priority="109">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="94">
-      <formula>O$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="81" priority="95">
+    <cfRule type="expression" dxfId="82" priority="110">
+      <formula>F$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="81" priority="111">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="96">
+    <cfRule type="expression" dxfId="80" priority="112">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S14">
-    <cfRule type="expression" dxfId="79" priority="49">
+  <conditionalFormatting sqref="Q14">
+    <cfRule type="expression" dxfId="79" priority="97">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="50">
+    <cfRule type="expression" dxfId="78" priority="98">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="51">
+    <cfRule type="expression" dxfId="77" priority="99">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="52">
+    <cfRule type="expression" dxfId="76" priority="100">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="53">
+    <cfRule type="expression" dxfId="75" priority="101">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="54">
+    <cfRule type="expression" dxfId="74" priority="102">
+      <formula>Q$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="73" priority="103">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="72" priority="104">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R14">
+    <cfRule type="expression" dxfId="71" priority="89">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="70" priority="90">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="69" priority="91">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="68" priority="92">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="67" priority="93">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="66" priority="94">
+      <formula>R$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="65" priority="95">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="96">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S15">
+    <cfRule type="expression" dxfId="63" priority="81">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="62" priority="82">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="61" priority="83">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="60" priority="84">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="85">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="58" priority="86">
       <formula>S$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="55">
+    <cfRule type="expression" dxfId="57" priority="87">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="56">
+    <cfRule type="expression" dxfId="56" priority="88">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
-    <cfRule type="expression" dxfId="71" priority="33">
+  <conditionalFormatting sqref="T15">
+    <cfRule type="expression" dxfId="55" priority="73">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="34">
+    <cfRule type="expression" dxfId="54" priority="74">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="35">
+    <cfRule type="expression" dxfId="53" priority="75">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="36">
+    <cfRule type="expression" dxfId="52" priority="76">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="37">
+    <cfRule type="expression" dxfId="51" priority="77">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="38">
-      <formula>H$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="65" priority="39">
+    <cfRule type="expression" dxfId="50" priority="78">
+      <formula>T$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="79">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="40">
+    <cfRule type="expression" dxfId="48" priority="80">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K12:L12">
-    <cfRule type="expression" dxfId="63" priority="25">
+  <conditionalFormatting sqref="V16">
+    <cfRule type="expression" dxfId="47" priority="65">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="26">
+    <cfRule type="expression" dxfId="46" priority="66">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="27">
+    <cfRule type="expression" dxfId="45" priority="67">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="28">
+    <cfRule type="expression" dxfId="44" priority="68">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="29">
+    <cfRule type="expression" dxfId="43" priority="69">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="30">
-      <formula>K$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="57" priority="31">
+    <cfRule type="expression" dxfId="42" priority="70">
+      <formula>V$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="71">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="32">
+    <cfRule type="expression" dxfId="40" priority="72">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X15">
-    <cfRule type="expression" dxfId="55" priority="81">
+  <conditionalFormatting sqref="W16">
+    <cfRule type="expression" dxfId="39" priority="57">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="82">
+    <cfRule type="expression" dxfId="38" priority="58">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="83">
+    <cfRule type="expression" dxfId="37" priority="59">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="84">
+    <cfRule type="expression" dxfId="36" priority="60">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="85">
+    <cfRule type="expression" dxfId="35" priority="61">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="86">
-      <formula>X$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="49" priority="87">
+    <cfRule type="expression" dxfId="34" priority="62">
+      <formula>W$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="63">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="88">
+    <cfRule type="expression" dxfId="32" priority="64">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W15">
-    <cfRule type="expression" dxfId="47" priority="73">
+  <conditionalFormatting sqref="U15">
+    <cfRule type="expression" dxfId="31" priority="49">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="74">
+    <cfRule type="expression" dxfId="30" priority="50">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="75">
+    <cfRule type="expression" dxfId="29" priority="51">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="76">
+    <cfRule type="expression" dxfId="28" priority="52">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="77">
+    <cfRule type="expression" dxfId="27" priority="53">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="78">
-      <formula>W$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="41" priority="79">
+    <cfRule type="expression" dxfId="26" priority="54">
+      <formula>U$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="55">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="80">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U16">
-    <cfRule type="expression" dxfId="39" priority="65">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="66">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="67">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="68">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="35" priority="69">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="34" priority="70">
-      <formula>U$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="33" priority="71">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="72">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q15">
-    <cfRule type="expression" dxfId="31" priority="41">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="30" priority="42">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="29" priority="43">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="44">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="45">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="46">
-      <formula>Q$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="47">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="48">
+    <cfRule type="expression" dxfId="24" priority="56">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4991,7 +5688,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F18:AD18 AF18:AM18">
+  <conditionalFormatting sqref="N13">
     <cfRule type="expression" dxfId="15" priority="9">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -5008,7 +5705,7 @@
       <formula>Plan</formula>
     </cfRule>
     <cfRule type="expression" dxfId="10" priority="14">
-      <formula>F$8=period_selected</formula>
+      <formula>N$8=period_selected</formula>
     </cfRule>
     <cfRule type="expression" dxfId="9" priority="15">
       <formula>MOD(COLUMN(),2)</formula>
@@ -5017,7 +5714,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20:AJ20 AL20:AM20">
+  <conditionalFormatting sqref="X16">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -5034,7 +5731,7 @@
       <formula>Plan</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="6">
-      <formula>F$8=period_selected</formula>
+      <formula>X$8=period_selected</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="7">
       <formula>MOD(COLUMN(),2)</formula>

</xml_diff>

<commit_message>
improved P2 document based on feedback
</commit_message>
<xml_diff>
--- a/Thesis Planning.xlsx
+++ b/Thesis Planning.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
   <si>
     <t>Plan</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>1 week</t>
-  </si>
-  <si>
-    <t>Prepare sensor data sets</t>
   </si>
   <si>
     <t>P4 Deadline</t>
@@ -149,7 +146,13 @@
     <t>Converting static data to RDF</t>
   </si>
   <si>
-    <t>2 weeks</t>
+    <t>Create WPS to publish linked data</t>
+  </si>
+  <si>
+    <t>Create WPS to query linked data</t>
+  </si>
+  <si>
+    <t>3 weeks</t>
   </si>
 </sst>
 </file>
@@ -418,7 +421,2493 @@
     <cellStyle name="Period Highlight Control" xfId="7"/>
     <cellStyle name="Project Headers" xfId="4"/>
   </cellStyles>
-  <dxfs count="258">
+  <dxfs count="434">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4316,10 +6805,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:AM33"/>
+  <dimension ref="A2:AM34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="O17" sqref="O17:S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -4357,7 +6846,7 @@
   <sheetData>
     <row r="2" spans="1:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -4413,7 +6902,7 @@
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -4585,13 +7074,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="16">
         <v>42317</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="9"/>
@@ -4604,1065 +7093,1608 @@
         <v>5</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" s="16">
         <v>42345</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
       <c r="O13" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="P13" s="7"/>
-      <c r="U13" s="7"/>
+        <v>24</v>
+      </c>
+      <c r="T13" s="7"/>
     </row>
     <row r="14" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>6</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C14" s="16">
         <v>42380</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
+      <c r="U14" s="7"/>
+      <c r="V14" s="7"/>
     </row>
     <row r="15" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>7</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C15" s="16">
         <v>42401</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>8</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
       <c r="V15" s="7"/>
       <c r="W15" s="7"/>
-      <c r="X15" s="7"/>
     </row>
     <row r="16" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>8</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="16">
         <v>42429</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>8</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="R16" s="7"/>
       <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
+      <c r="X16" s="7"/>
       <c r="Y16" s="7"/>
-      <c r="Z16" s="7"/>
-      <c r="AA16" s="7"/>
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
     </row>
-    <row r="17" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>9</v>
       </c>
-      <c r="B17" s="14" t="s">
-        <v>29</v>
+      <c r="B17" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="C17" s="16">
-        <v>42394</v>
+        <v>42408</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
+        <v>25</v>
+      </c>
       <c r="S17" s="7"/>
-      <c r="T17" s="7"/>
-      <c r="U17" s="7"/>
-      <c r="V17" s="7"/>
-      <c r="W17" s="7"/>
-      <c r="X17" s="7"/>
       <c r="Y17" s="7"/>
       <c r="Z17" s="7"/>
-      <c r="AA17" s="7"/>
-      <c r="AB17" s="7"/>
-      <c r="AC17" s="7"/>
-      <c r="AD17" s="7"/>
+      <c r="AA17" s="1"/>
+      <c r="AC17" s="1"/>
+      <c r="AE17" s="1"/>
+      <c r="AG17" s="1"/>
+      <c r="AI17" s="1"/>
+      <c r="AK17" s="1"/>
+      <c r="AM17" s="1"/>
     </row>
-    <row r="18" spans="1:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>10</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C18" s="16">
-        <v>42492</v>
+        <v>42394</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="AE18" s="7"/>
+        <v>33</v>
+      </c>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="7"/>
+      <c r="AA18" s="7"/>
+      <c r="AB18" s="7"/>
+      <c r="AC18" s="7"/>
+      <c r="AD18" s="7"/>
     </row>
-    <row r="19" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:39" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>11</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C19" s="16">
-        <v>42499</v>
+        <v>42492</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF19" s="7"/>
-      <c r="AG19" s="7"/>
-      <c r="AH19" s="7"/>
-      <c r="AI19" s="7"/>
-      <c r="AJ19" s="7"/>
+        <v>17</v>
+      </c>
+      <c r="AE19" s="7"/>
     </row>
-    <row r="20" spans="1:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>12</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C20" s="16">
+        <v>42499</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF20" s="7"/>
+      <c r="AG20" s="7"/>
+      <c r="AH20" s="7"/>
+      <c r="AI20" s="7"/>
+      <c r="AJ20" s="7"/>
+    </row>
+    <row r="21" spans="1:39" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>13</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="16">
         <v>42534</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D21" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="AK20" s="7"/>
+      <c r="AK21" s="7"/>
     </row>
-    <row r="21" spans="1:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="10"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="11"/>
+    <row r="22" spans="1:39" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="10"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="11"/>
     </row>
-    <row r="22" spans="1:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="14" t="s">
+    <row r="23" spans="1:39" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="16">
+      <c r="C23" s="16">
         <v>42318</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="16">
-        <v>42379</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="N23" s="8"/>
+      <c r="F23" s="8"/>
     </row>
-    <row r="24" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C24" s="16">
-        <v>42387</v>
+        <v>42379</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="P24" s="7"/>
+      <c r="N24" s="8"/>
     </row>
-    <row r="25" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>21</v>
+        <v>14</v>
+      </c>
+      <c r="C25" s="16">
+        <v>42387</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>6</v>
       </c>
+      <c r="P25" s="7"/>
     </row>
-    <row r="26" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="16">
-        <v>42126</v>
+      <c r="C26" s="18" t="s">
+        <v>20</v>
       </c>
       <c r="D26" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="AD26" s="7"/>
     </row>
-    <row r="27" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="14" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C27" s="16">
-        <v>42133</v>
+        <v>42126</v>
       </c>
       <c r="D27" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="AF27" s="7"/>
+      <c r="AD27" s="7"/>
     </row>
-    <row r="28" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C28" s="16">
-        <v>42168</v>
+        <v>42133</v>
       </c>
       <c r="D28" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="AJ28" s="7"/>
+      <c r="AF28" s="7"/>
     </row>
-    <row r="29" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C29" s="16">
-        <v>42175</v>
+        <v>42168</v>
       </c>
       <c r="D29" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="AK29" t="s">
-        <v>25</v>
-      </c>
-      <c r="AL29" s="7"/>
+      <c r="AJ29" s="7"/>
     </row>
-    <row r="30" spans="1:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="10"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="11"/>
+    <row r="30" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="16">
+        <v>42175</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="AK30" t="s">
+        <v>24</v>
+      </c>
+      <c r="AL30" s="7"/>
     </row>
-    <row r="31" spans="1:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="16">
+    <row r="31" spans="1:39" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="10"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="11"/>
+    </row>
+    <row r="32" spans="1:39" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="16">
         <v>42325</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="D32" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G31" s="8"/>
+      <c r="G32" s="8"/>
     </row>
-    <row r="32" spans="1:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="14" t="s">
+    <row r="33" spans="2:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="16">
+      <c r="C33" s="16">
         <v>42361</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D33" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
     </row>
-    <row r="33" spans="2:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="14"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="15"/>
+    <row r="34" spans="2:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="14"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:D4"/>
   </mergeCells>
-  <conditionalFormatting sqref="G22:AM22 F31 H31:O31 F32:K33 N32:AM33 O10:AM10 T13 P23:AM23 F23:H23 F24:O29 Q28:AI28 Q26:AC26 Q27:AE27 Q29:AK29 J33:Q33 Q24:AM25 AF26:AM26 AG27:AM27 AM29 AL28:AM28 F21:AM21 Q30:AM31 P11:AM11 P19:AE19 AK19:AM19 P17 P15 P16:R16 Y15:AM15 AB16:AM16 AE17:AM17 M9:AM9 M12:AM12 F15:N17 F11:N11 F19:N19 V13:AM14">
-    <cfRule type="expression" dxfId="257" priority="401">
+  <conditionalFormatting sqref="G23:AM23 F32 H32:O32 F33:K34 N33:AM34 O10:AM10 P24:AM24 F24:H24 F25:O30 Q29:AI29 Q27:AC27 Q28:AE28 Q30:AK30 J34:Q34 Q25:AM26 AF27:AM27 AG28:AM28 AM30 AL29:AM29 F22:AM22 Q31:AM32 P11:AM11 P20:AE20 AK20:AM20 Y15:AM15 AB16:AM16 AE18:AM18 M9:AM9 M12:AM12 F15:N15 F11:N11 F20:N20 V13:AM13 W14:AM14 F18:P18 F16:R16">
+    <cfRule type="expression" dxfId="433" priority="601">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="256" priority="403">
+    <cfRule type="expression" dxfId="432" priority="603">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="255" priority="404">
+    <cfRule type="expression" dxfId="431" priority="604">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="254" priority="405">
+    <cfRule type="expression" dxfId="430" priority="605">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="253" priority="406">
+    <cfRule type="expression" dxfId="429" priority="606">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="252" priority="407">
+    <cfRule type="expression" dxfId="428" priority="607">
       <formula>F$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="251" priority="411">
+    <cfRule type="expression" dxfId="427" priority="611">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="250" priority="412">
+    <cfRule type="expression" dxfId="426" priority="612">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B34:AM34">
-    <cfRule type="expression" dxfId="249" priority="402">
+  <conditionalFormatting sqref="B35:AM35">
+    <cfRule type="expression" dxfId="425" priority="602">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8:AM8">
-    <cfRule type="expression" dxfId="248" priority="408">
+    <cfRule type="expression" dxfId="424" priority="608">
       <formula>F$8=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="expression" dxfId="247" priority="377">
+    <cfRule type="expression" dxfId="423" priority="577">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="246" priority="378">
+    <cfRule type="expression" dxfId="422" priority="578">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="245" priority="379">
+    <cfRule type="expression" dxfId="421" priority="579">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="244" priority="380">
+    <cfRule type="expression" dxfId="420" priority="580">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="243" priority="381">
+    <cfRule type="expression" dxfId="419" priority="581">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="242" priority="382">
+    <cfRule type="expression" dxfId="418" priority="582">
       <formula>G$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="241" priority="383">
+    <cfRule type="expression" dxfId="417" priority="583">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="240" priority="384">
+    <cfRule type="expression" dxfId="416" priority="584">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="expression" dxfId="239" priority="369">
+    <cfRule type="expression" dxfId="415" priority="569">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="238" priority="370">
+    <cfRule type="expression" dxfId="414" priority="570">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="237" priority="371">
+    <cfRule type="expression" dxfId="413" priority="571">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="236" priority="372">
+    <cfRule type="expression" dxfId="412" priority="572">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="235" priority="373">
+    <cfRule type="expression" dxfId="411" priority="573">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="234" priority="374">
+    <cfRule type="expression" dxfId="410" priority="574">
       <formula>F$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="233" priority="375">
+    <cfRule type="expression" dxfId="409" priority="575">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="232" priority="376">
+    <cfRule type="expression" dxfId="408" priority="576">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I23:M23">
-    <cfRule type="expression" dxfId="231" priority="329">
+  <conditionalFormatting sqref="I24:M24">
+    <cfRule type="expression" dxfId="407" priority="529">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="230" priority="330">
+    <cfRule type="expression" dxfId="406" priority="530">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="229" priority="331">
+    <cfRule type="expression" dxfId="405" priority="531">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="228" priority="332">
+    <cfRule type="expression" dxfId="404" priority="532">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="227" priority="333">
+    <cfRule type="expression" dxfId="403" priority="533">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="226" priority="334">
+    <cfRule type="expression" dxfId="402" priority="534">
       <formula>I$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="225" priority="335">
+    <cfRule type="expression" dxfId="401" priority="535">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="224" priority="336">
+    <cfRule type="expression" dxfId="400" priority="536">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O23">
-    <cfRule type="expression" dxfId="223" priority="321">
+  <conditionalFormatting sqref="O24">
+    <cfRule type="expression" dxfId="399" priority="521">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="222" priority="322">
+    <cfRule type="expression" dxfId="398" priority="522">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="221" priority="323">
+    <cfRule type="expression" dxfId="397" priority="523">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="220" priority="324">
+    <cfRule type="expression" dxfId="396" priority="524">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="219" priority="325">
+    <cfRule type="expression" dxfId="395" priority="525">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="218" priority="326">
+    <cfRule type="expression" dxfId="394" priority="526">
       <formula>O$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="217" priority="327">
+    <cfRule type="expression" dxfId="393" priority="527">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="216" priority="328">
+    <cfRule type="expression" dxfId="392" priority="528">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14:J14 F13:I13">
-    <cfRule type="expression" dxfId="215" priority="305">
+    <cfRule type="expression" dxfId="391" priority="505">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="214" priority="306">
+    <cfRule type="expression" dxfId="390" priority="506">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="213" priority="307">
+    <cfRule type="expression" dxfId="389" priority="507">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="212" priority="308">
+    <cfRule type="expression" dxfId="388" priority="508">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="211" priority="309">
+    <cfRule type="expression" dxfId="387" priority="509">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="210" priority="310">
+    <cfRule type="expression" dxfId="386" priority="510">
       <formula>F$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="209" priority="311">
+    <cfRule type="expression" dxfId="385" priority="511">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="208" priority="312">
+    <cfRule type="expression" dxfId="384" priority="512">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14:N14">
-    <cfRule type="expression" dxfId="207" priority="297">
+    <cfRule type="expression" dxfId="383" priority="497">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="206" priority="298">
+    <cfRule type="expression" dxfId="382" priority="498">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="205" priority="299">
+    <cfRule type="expression" dxfId="381" priority="499">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="204" priority="300">
+    <cfRule type="expression" dxfId="380" priority="500">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="203" priority="301">
+    <cfRule type="expression" dxfId="379" priority="501">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="202" priority="302">
+    <cfRule type="expression" dxfId="378" priority="502">
       <formula>K$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="201" priority="303">
+    <cfRule type="expression" dxfId="377" priority="503">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="200" priority="304">
+    <cfRule type="expression" dxfId="376" priority="504">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F30:O30">
-    <cfRule type="expression" dxfId="199" priority="281">
+  <conditionalFormatting sqref="F31:O31">
+    <cfRule type="expression" dxfId="375" priority="481">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="198" priority="282">
+    <cfRule type="expression" dxfId="374" priority="482">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="197" priority="283">
+    <cfRule type="expression" dxfId="373" priority="483">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="196" priority="284">
+    <cfRule type="expression" dxfId="372" priority="484">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="195" priority="285">
+    <cfRule type="expression" dxfId="371" priority="485">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="194" priority="286">
+    <cfRule type="expression" dxfId="370" priority="486">
       <formula>F$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="193" priority="287">
+    <cfRule type="expression" dxfId="369" priority="487">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="192" priority="288">
+    <cfRule type="expression" dxfId="368" priority="488">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P25:P27">
-    <cfRule type="expression" dxfId="191" priority="273">
+  <conditionalFormatting sqref="P26:P28">
+    <cfRule type="expression" dxfId="367" priority="473">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="190" priority="274">
+    <cfRule type="expression" dxfId="366" priority="474">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="189" priority="275">
+    <cfRule type="expression" dxfId="365" priority="475">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="188" priority="276">
+    <cfRule type="expression" dxfId="364" priority="476">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="187" priority="277">
+    <cfRule type="expression" dxfId="363" priority="477">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="186" priority="278">
+    <cfRule type="expression" dxfId="362" priority="478">
       <formula>P$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="185" priority="279">
+    <cfRule type="expression" dxfId="361" priority="479">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="184" priority="280">
+    <cfRule type="expression" dxfId="360" priority="480">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P28:P31">
-    <cfRule type="expression" dxfId="183" priority="265">
+  <conditionalFormatting sqref="P29:P32">
+    <cfRule type="expression" dxfId="359" priority="465">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="182" priority="266">
+    <cfRule type="expression" dxfId="358" priority="466">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="181" priority="267">
+    <cfRule type="expression" dxfId="357" priority="467">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="180" priority="268">
+    <cfRule type="expression" dxfId="356" priority="468">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="179" priority="269">
+    <cfRule type="expression" dxfId="355" priority="469">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="178" priority="270">
+    <cfRule type="expression" dxfId="354" priority="470">
       <formula>P$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="177" priority="271">
+    <cfRule type="expression" dxfId="353" priority="471">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="176" priority="272">
+    <cfRule type="expression" dxfId="352" priority="472">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE26">
-    <cfRule type="expression" dxfId="175" priority="257">
+  <conditionalFormatting sqref="AE27">
+    <cfRule type="expression" dxfId="351" priority="457">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="174" priority="258">
+    <cfRule type="expression" dxfId="350" priority="458">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="173" priority="259">
+    <cfRule type="expression" dxfId="349" priority="459">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="172" priority="260">
+    <cfRule type="expression" dxfId="348" priority="460">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="171" priority="261">
+    <cfRule type="expression" dxfId="347" priority="461">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="170" priority="262">
+    <cfRule type="expression" dxfId="346" priority="462">
       <formula>AE$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="169" priority="263">
+    <cfRule type="expression" dxfId="345" priority="463">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="168" priority="264">
+    <cfRule type="expression" dxfId="344" priority="464">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK28">
-    <cfRule type="expression" dxfId="167" priority="249">
+  <conditionalFormatting sqref="AK29">
+    <cfRule type="expression" dxfId="343" priority="449">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="166" priority="250">
+    <cfRule type="expression" dxfId="342" priority="450">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="165" priority="251">
+    <cfRule type="expression" dxfId="341" priority="451">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="164" priority="252">
+    <cfRule type="expression" dxfId="340" priority="452">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="163" priority="253">
+    <cfRule type="expression" dxfId="339" priority="453">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="162" priority="254">
+    <cfRule type="expression" dxfId="338" priority="454">
       <formula>AK$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="161" priority="255">
+    <cfRule type="expression" dxfId="337" priority="455">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="160" priority="256">
+    <cfRule type="expression" dxfId="336" priority="456">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q13:S13">
-    <cfRule type="expression" dxfId="159" priority="241">
+    <cfRule type="expression" dxfId="335" priority="441">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="158" priority="242">
+    <cfRule type="expression" dxfId="334" priority="442">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="157" priority="243">
+    <cfRule type="expression" dxfId="333" priority="443">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="156" priority="244">
+    <cfRule type="expression" dxfId="332" priority="444">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="155" priority="245">
+    <cfRule type="expression" dxfId="331" priority="445">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="154" priority="246">
+    <cfRule type="expression" dxfId="330" priority="446">
       <formula>Q$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="153" priority="247">
+    <cfRule type="expression" dxfId="329" priority="447">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="152" priority="248">
+    <cfRule type="expression" dxfId="328" priority="448">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T14:U14">
-    <cfRule type="expression" dxfId="151" priority="233">
+  <conditionalFormatting sqref="T14">
+    <cfRule type="expression" dxfId="327" priority="433">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="150" priority="234">
+    <cfRule type="expression" dxfId="326" priority="434">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="149" priority="235">
+    <cfRule type="expression" dxfId="325" priority="435">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="148" priority="236">
+    <cfRule type="expression" dxfId="324" priority="436">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="147" priority="237">
+    <cfRule type="expression" dxfId="323" priority="437">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="146" priority="238">
+    <cfRule type="expression" dxfId="322" priority="438">
       <formula>T$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="145" priority="239">
+    <cfRule type="expression" dxfId="321" priority="439">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="144" priority="240">
+    <cfRule type="expression" dxfId="320" priority="440">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9">
-    <cfRule type="expression" dxfId="143" priority="225">
+    <cfRule type="expression" dxfId="319" priority="425">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="142" priority="226">
+    <cfRule type="expression" dxfId="318" priority="426">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="141" priority="227">
+    <cfRule type="expression" dxfId="317" priority="427">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="140" priority="228">
+    <cfRule type="expression" dxfId="316" priority="428">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="139" priority="229">
+    <cfRule type="expression" dxfId="315" priority="429">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="138" priority="230">
+    <cfRule type="expression" dxfId="314" priority="430">
       <formula>L$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="137" priority="231">
+    <cfRule type="expression" dxfId="313" priority="431">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="136" priority="232">
+    <cfRule type="expression" dxfId="312" priority="432">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O15:O17 O19">
-    <cfRule type="expression" dxfId="135" priority="193">
+  <conditionalFormatting sqref="O15 O20">
+    <cfRule type="expression" dxfId="311" priority="393">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="134" priority="194">
+    <cfRule type="expression" dxfId="310" priority="394">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="133" priority="195">
+    <cfRule type="expression" dxfId="309" priority="395">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="132" priority="196">
+    <cfRule type="expression" dxfId="308" priority="396">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="131" priority="197">
+    <cfRule type="expression" dxfId="307" priority="397">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="130" priority="198">
+    <cfRule type="expression" dxfId="306" priority="398">
       <formula>O$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="129" priority="199">
+    <cfRule type="expression" dxfId="305" priority="399">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="128" priority="200">
+    <cfRule type="expression" dxfId="304" priority="400">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S14">
-    <cfRule type="expression" dxfId="127" priority="153">
+    <cfRule type="expression" dxfId="303" priority="353">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="126" priority="154">
+    <cfRule type="expression" dxfId="302" priority="354">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="155">
+    <cfRule type="expression" dxfId="301" priority="355">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="156">
+    <cfRule type="expression" dxfId="300" priority="356">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="157">
+    <cfRule type="expression" dxfId="299" priority="357">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="158">
+    <cfRule type="expression" dxfId="298" priority="358">
       <formula>S$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="121" priority="159">
+    <cfRule type="expression" dxfId="297" priority="359">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="120" priority="160">
+    <cfRule type="expression" dxfId="296" priority="360">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="expression" dxfId="119" priority="137">
+    <cfRule type="expression" dxfId="295" priority="337">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="138">
+    <cfRule type="expression" dxfId="294" priority="338">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="139">
+    <cfRule type="expression" dxfId="293" priority="339">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="140">
+    <cfRule type="expression" dxfId="292" priority="340">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="141">
+    <cfRule type="expression" dxfId="291" priority="341">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="142">
+    <cfRule type="expression" dxfId="290" priority="342">
       <formula>H$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="143">
+    <cfRule type="expression" dxfId="289" priority="343">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="144">
+    <cfRule type="expression" dxfId="288" priority="344">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12:L12">
-    <cfRule type="expression" dxfId="111" priority="129">
+    <cfRule type="expression" dxfId="287" priority="329">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="130">
+    <cfRule type="expression" dxfId="286" priority="330">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="131">
+    <cfRule type="expression" dxfId="285" priority="331">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="132">
+    <cfRule type="expression" dxfId="284" priority="332">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="133">
+    <cfRule type="expression" dxfId="283" priority="333">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="134">
+    <cfRule type="expression" dxfId="282" priority="334">
       <formula>K$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="135">
+    <cfRule type="expression" dxfId="281" priority="335">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="136">
+    <cfRule type="expression" dxfId="280" priority="336">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U16">
-    <cfRule type="expression" dxfId="103" priority="169">
+    <cfRule type="expression" dxfId="279" priority="369">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="170">
+    <cfRule type="expression" dxfId="278" priority="370">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="171">
+    <cfRule type="expression" dxfId="277" priority="371">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="172">
+    <cfRule type="expression" dxfId="276" priority="372">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="173">
+    <cfRule type="expression" dxfId="275" priority="373">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="174">
+    <cfRule type="expression" dxfId="274" priority="374">
       <formula>U$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="175">
+    <cfRule type="expression" dxfId="273" priority="375">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="176">
+    <cfRule type="expression" dxfId="272" priority="376">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F18:AD18 AF18:AM18">
-    <cfRule type="expression" dxfId="95" priority="113">
+  <conditionalFormatting sqref="F19:AD19 AF19:AM19">
+    <cfRule type="expression" dxfId="271" priority="313">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="114">
+    <cfRule type="expression" dxfId="270" priority="314">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="115">
+    <cfRule type="expression" dxfId="269" priority="315">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="116">
+    <cfRule type="expression" dxfId="268" priority="316">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="117">
+    <cfRule type="expression" dxfId="267" priority="317">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="118">
+    <cfRule type="expression" dxfId="266" priority="318">
       <formula>F$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="119">
+    <cfRule type="expression" dxfId="265" priority="319">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="120">
+    <cfRule type="expression" dxfId="264" priority="320">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20:AJ20 AL20:AM20">
-    <cfRule type="expression" dxfId="87" priority="105">
+  <conditionalFormatting sqref="F21:AJ21 AL21:AM21">
+    <cfRule type="expression" dxfId="263" priority="305">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="106">
+    <cfRule type="expression" dxfId="262" priority="306">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="107">
+    <cfRule type="expression" dxfId="261" priority="307">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="108">
+    <cfRule type="expression" dxfId="260" priority="308">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="109">
+    <cfRule type="expression" dxfId="259" priority="309">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="110">
+    <cfRule type="expression" dxfId="258" priority="310">
       <formula>F$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="111">
+    <cfRule type="expression" dxfId="257" priority="311">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="112">
+    <cfRule type="expression" dxfId="256" priority="312">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q14">
-    <cfRule type="expression" dxfId="79" priority="97">
+    <cfRule type="expression" dxfId="255" priority="297">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="98">
+    <cfRule type="expression" dxfId="254" priority="298">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="99">
+    <cfRule type="expression" dxfId="253" priority="299">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="100">
+    <cfRule type="expression" dxfId="252" priority="300">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="101">
+    <cfRule type="expression" dxfId="251" priority="301">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="102">
+    <cfRule type="expression" dxfId="250" priority="302">
       <formula>Q$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="103">
+    <cfRule type="expression" dxfId="249" priority="303">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="104">
+    <cfRule type="expression" dxfId="248" priority="304">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R14">
-    <cfRule type="expression" dxfId="71" priority="89">
+    <cfRule type="expression" dxfId="247" priority="289">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="90">
+    <cfRule type="expression" dxfId="246" priority="290">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="91">
+    <cfRule type="expression" dxfId="245" priority="291">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="92">
+    <cfRule type="expression" dxfId="244" priority="292">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="93">
+    <cfRule type="expression" dxfId="243" priority="293">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="94">
+    <cfRule type="expression" dxfId="242" priority="294">
       <formula>R$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="95">
+    <cfRule type="expression" dxfId="241" priority="295">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="96">
+    <cfRule type="expression" dxfId="240" priority="296">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S15">
-    <cfRule type="expression" dxfId="63" priority="81">
+    <cfRule type="expression" dxfId="239" priority="281">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="82">
+    <cfRule type="expression" dxfId="238" priority="282">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="83">
+    <cfRule type="expression" dxfId="237" priority="283">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="84">
+    <cfRule type="expression" dxfId="236" priority="284">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="85">
+    <cfRule type="expression" dxfId="235" priority="285">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="86">
+    <cfRule type="expression" dxfId="234" priority="286">
       <formula>S$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="87">
+    <cfRule type="expression" dxfId="233" priority="287">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="88">
+    <cfRule type="expression" dxfId="232" priority="288">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T15">
-    <cfRule type="expression" dxfId="55" priority="73">
+    <cfRule type="expression" dxfId="231" priority="273">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="74">
+    <cfRule type="expression" dxfId="230" priority="274">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="75">
+    <cfRule type="expression" dxfId="229" priority="275">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="76">
+    <cfRule type="expression" dxfId="228" priority="276">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="77">
+    <cfRule type="expression" dxfId="227" priority="277">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="78">
+    <cfRule type="expression" dxfId="226" priority="278">
       <formula>T$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="79">
+    <cfRule type="expression" dxfId="225" priority="279">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="80">
+    <cfRule type="expression" dxfId="224" priority="280">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V16">
-    <cfRule type="expression" dxfId="47" priority="65">
+    <cfRule type="expression" dxfId="223" priority="265">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="66">
+    <cfRule type="expression" dxfId="222" priority="266">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="67">
+    <cfRule type="expression" dxfId="221" priority="267">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="68">
+    <cfRule type="expression" dxfId="220" priority="268">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="69">
+    <cfRule type="expression" dxfId="219" priority="269">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="70">
+    <cfRule type="expression" dxfId="218" priority="270">
       <formula>V$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="71">
+    <cfRule type="expression" dxfId="217" priority="271">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="72">
+    <cfRule type="expression" dxfId="216" priority="272">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W16">
-    <cfRule type="expression" dxfId="39" priority="57">
+    <cfRule type="expression" dxfId="215" priority="257">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="58">
+    <cfRule type="expression" dxfId="214" priority="258">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="59">
+    <cfRule type="expression" dxfId="213" priority="259">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="60">
+    <cfRule type="expression" dxfId="212" priority="260">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="61">
+    <cfRule type="expression" dxfId="211" priority="261">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="62">
+    <cfRule type="expression" dxfId="210" priority="262">
       <formula>W$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="63">
+    <cfRule type="expression" dxfId="209" priority="263">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="64">
+    <cfRule type="expression" dxfId="208" priority="264">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U15">
-    <cfRule type="expression" dxfId="31" priority="49">
+    <cfRule type="expression" dxfId="207" priority="249">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="50">
+    <cfRule type="expression" dxfId="206" priority="250">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="51">
+    <cfRule type="expression" dxfId="205" priority="251">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="52">
+    <cfRule type="expression" dxfId="204" priority="252">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="53">
+    <cfRule type="expression" dxfId="203" priority="253">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="54">
+    <cfRule type="expression" dxfId="202" priority="254">
       <formula>U$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="55">
+    <cfRule type="expression" dxfId="201" priority="255">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="56">
+    <cfRule type="expression" dxfId="200" priority="256">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T16">
+    <cfRule type="expression" dxfId="199" priority="177">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="198" priority="178">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="197" priority="179">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="196" priority="180">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="195" priority="181">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="194" priority="182">
+      <formula>T$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="193" priority="183">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="192" priority="184">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N13">
+    <cfRule type="expression" dxfId="191" priority="209">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="190" priority="210">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="189" priority="211">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="188" priority="212">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="187" priority="213">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="186" priority="214">
+      <formula>N$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="185" priority="215">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="184" priority="216">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X15">
+    <cfRule type="expression" dxfId="183" priority="161">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="182" priority="162">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="181" priority="163">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="180" priority="164">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="179" priority="165">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="178" priority="166">
+      <formula>X$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="177" priority="167">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="176" priority="168">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R15">
+    <cfRule type="expression" dxfId="167" priority="185">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="166" priority="186">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="165" priority="187">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="164" priority="188">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="163" priority="189">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="162" priority="190">
+      <formula>R$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="161" priority="191">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="160" priority="192">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA16">
+    <cfRule type="expression" dxfId="159" priority="169">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="158" priority="170">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="157" priority="171">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="156" priority="172">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="155" priority="173">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="154" priority="174">
+      <formula>AA$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="153" priority="175">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="152" priority="176">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U13">
+    <cfRule type="expression" dxfId="151" priority="145">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="150" priority="146">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="149" priority="147">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="148" priority="148">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="147" priority="149">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="146" priority="150">
+      <formula>U$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="145" priority="151">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="144" priority="152">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P13">
+    <cfRule type="expression" dxfId="143" priority="137">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="142" priority="138">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="141" priority="139">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="140" priority="140">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="139" priority="141">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="138" priority="142">
+      <formula>P$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="137" priority="143">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="136" priority="144">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G17">
+    <cfRule type="expression" dxfId="135" priority="129">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="134" priority="130">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="133" priority="131">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="132" priority="132">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="131" priority="133">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="130" priority="134">
+      <formula>G$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="129" priority="135">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="128" priority="136">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17">
+    <cfRule type="expression" dxfId="127" priority="121">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="126" priority="122">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="125" priority="123">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="124" priority="124">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="123" priority="125">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="122" priority="126">
+      <formula>I$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="121" priority="127">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="120" priority="128">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K17">
+    <cfRule type="expression" dxfId="119" priority="113">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="118" priority="114">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="117" priority="115">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="116" priority="116">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="115" priority="117">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="114" priority="118">
+      <formula>K$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="113" priority="119">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="112" priority="120">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M17">
+    <cfRule type="expression" dxfId="111" priority="105">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="110" priority="106">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="109" priority="107">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="108" priority="108">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="107" priority="109">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="106" priority="110">
+      <formula>M$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="105" priority="111">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="104" priority="112">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O17">
+    <cfRule type="expression" dxfId="103" priority="97">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="102" priority="98">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="101" priority="99">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="100" priority="100">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="99" priority="101">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="98" priority="102">
+      <formula>O$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="97" priority="103">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="96" priority="104">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q17">
+    <cfRule type="expression" dxfId="95" priority="89">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="94" priority="90">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="93" priority="91">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="92" priority="92">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="91" priority="93">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="90" priority="94">
+      <formula>Q$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="89" priority="95">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="88" priority="96">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U17">
+    <cfRule type="expression" dxfId="79" priority="73">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="78" priority="74">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="77" priority="75">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="76" priority="76">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="75" priority="77">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="74" priority="78">
+      <formula>U$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="73" priority="79">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="72" priority="80">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W17">
+    <cfRule type="expression" dxfId="71" priority="65">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="70" priority="66">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="69" priority="67">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="68" priority="68">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="67" priority="69">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="66" priority="70">
+      <formula>W$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="65" priority="71">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="72">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA17">
+    <cfRule type="expression" dxfId="63" priority="57">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="62" priority="58">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="61" priority="59">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="60" priority="60">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="61">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="58" priority="62">
+      <formula>AA$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="57" priority="63">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="56" priority="64">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC17">
+    <cfRule type="expression" dxfId="55" priority="49">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="50">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="53" priority="51">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="52" priority="52">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="51" priority="53">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="50" priority="54">
+      <formula>AC$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="55">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="56">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE17">
+    <cfRule type="expression" dxfId="47" priority="41">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="42">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="43">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="44">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="45">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="46">
+      <formula>AE$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="47">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="48">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG17">
+    <cfRule type="expression" dxfId="39" priority="33">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="34">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="35">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="36">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="37">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="38">
+      <formula>AG$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="39">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="40">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI17">
+    <cfRule type="expression" dxfId="31" priority="25">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="26">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="27">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="28">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="29">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="30">
+      <formula>AI$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="31">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="32">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK17">
     <cfRule type="expression" dxfId="23" priority="17">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -5679,7 +8711,7 @@
       <formula>Plan</formula>
     </cfRule>
     <cfRule type="expression" dxfId="18" priority="22">
-      <formula>AA$8=period_selected</formula>
+      <formula>AK$8=period_selected</formula>
     </cfRule>
     <cfRule type="expression" dxfId="17" priority="23">
       <formula>MOD(COLUMN(),2)</formula>
@@ -5688,7 +8720,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N13">
+  <conditionalFormatting sqref="AM17">
     <cfRule type="expression" dxfId="15" priority="9">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -5705,7 +8737,7 @@
       <formula>Plan</formula>
     </cfRule>
     <cfRule type="expression" dxfId="10" priority="14">
-      <formula>N$8=period_selected</formula>
+      <formula>AM$8=period_selected</formula>
     </cfRule>
     <cfRule type="expression" dxfId="9" priority="15">
       <formula>MOD(COLUMN(),2)</formula>
@@ -5714,7 +8746,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X16">
+  <conditionalFormatting sqref="Z16">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -5731,7 +8763,7 @@
       <formula>Plan</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="6">
-      <formula>X$8=period_selected</formula>
+      <formula>Z$8=period_selected</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="7">
       <formula>MOD(COLUMN(),2)</formula>

</xml_diff>

<commit_message>
improved P2 based on peer review feedback
</commit_message>
<xml_diff>
--- a/Thesis Planning.xlsx
+++ b/Thesis Planning.xlsx
@@ -389,9 +389,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="3" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
@@ -410,6 +407,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="3" xfId="3" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Activity" xfId="2"/>
@@ -421,233 +421,7 @@
     <cellStyle name="Period Highlight Control" xfId="7"/>
     <cellStyle name="Project Headers" xfId="4"/>
   </cellStyles>
-  <dxfs count="434">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="418">
     <dxf>
       <fill>
         <patternFill>
@@ -6808,7 +6582,7 @@
   <dimension ref="A2:AM34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17:S17"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -6837,24 +6611,20 @@
     <col min="25" max="25" width="6.75" style="1" customWidth="1"/>
     <col min="26" max="26" width="6.5" customWidth="1"/>
     <col min="27" max="27" width="6" customWidth="1"/>
-    <col min="28" max="30" width="6" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="33" max="35" width="6" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="37" max="39" width="6" bestFit="1" customWidth="1"/>
+    <col min="28" max="39" width="7.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:39" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="1:39" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
       <c r="F3" s="4"/>
       <c r="AA3" s="12"/>
       <c r="AD3" s="1"/>
@@ -6865,9 +6635,9 @@
       <c r="AI3" s="6"/>
     </row>
     <row r="4" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
       <c r="H4" s="7"/>
       <c r="I4" s="12" t="s">
         <v>0</v>
@@ -6911,120 +6681,120 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="13">
-        <v>42317</v>
-      </c>
-      <c r="G8" s="13">
-        <v>42324</v>
-      </c>
-      <c r="H8" s="13">
-        <v>42331</v>
-      </c>
-      <c r="I8" s="13">
-        <v>42338</v>
-      </c>
-      <c r="J8" s="13">
-        <v>42345</v>
-      </c>
-      <c r="K8" s="13">
-        <v>42352</v>
-      </c>
-      <c r="L8" s="13">
-        <v>42359</v>
-      </c>
-      <c r="M8" s="13">
-        <v>42366</v>
-      </c>
-      <c r="N8" s="13">
-        <v>42373</v>
-      </c>
-      <c r="O8" s="13">
-        <v>42380</v>
-      </c>
-      <c r="P8" s="13">
-        <v>42387</v>
-      </c>
-      <c r="Q8" s="13">
-        <v>42394</v>
-      </c>
-      <c r="R8" s="13">
-        <v>42401</v>
-      </c>
-      <c r="S8" s="13">
-        <v>42408</v>
-      </c>
-      <c r="T8" s="13">
-        <v>42415</v>
-      </c>
-      <c r="U8" s="13">
-        <v>42422</v>
-      </c>
-      <c r="V8" s="13">
-        <v>42429</v>
-      </c>
-      <c r="W8" s="13">
-        <v>42436</v>
-      </c>
-      <c r="X8" s="13">
-        <v>42443</v>
-      </c>
-      <c r="Y8" s="13">
-        <v>42450</v>
-      </c>
-      <c r="Z8" s="13">
-        <v>42457</v>
-      </c>
-      <c r="AA8" s="13">
-        <v>42464</v>
-      </c>
-      <c r="AB8" s="13">
-        <v>42471</v>
-      </c>
-      <c r="AC8" s="13">
-        <v>42478</v>
-      </c>
-      <c r="AD8" s="13">
-        <v>42485</v>
-      </c>
-      <c r="AE8" s="13">
-        <v>42492</v>
-      </c>
-      <c r="AF8" s="13">
-        <v>42499</v>
-      </c>
-      <c r="AG8" s="13">
-        <v>42506</v>
-      </c>
-      <c r="AH8" s="13">
-        <v>42513</v>
-      </c>
-      <c r="AI8" s="13">
-        <v>42520</v>
-      </c>
-      <c r="AJ8" s="13">
-        <v>42527</v>
-      </c>
-      <c r="AK8" s="13">
-        <v>42534</v>
-      </c>
-      <c r="AL8" s="13">
-        <v>42541</v>
-      </c>
-      <c r="AM8" s="13">
-        <v>42548</v>
+      <c r="F8" s="19">
+        <v>46</v>
+      </c>
+      <c r="G8" s="19">
+        <v>47</v>
+      </c>
+      <c r="H8" s="19">
+        <v>48</v>
+      </c>
+      <c r="I8" s="19">
+        <v>49</v>
+      </c>
+      <c r="J8" s="19">
+        <v>50</v>
+      </c>
+      <c r="K8" s="19">
+        <v>51</v>
+      </c>
+      <c r="L8" s="19">
+        <v>52</v>
+      </c>
+      <c r="M8" s="19">
+        <v>53</v>
+      </c>
+      <c r="N8" s="19">
+        <v>1</v>
+      </c>
+      <c r="O8" s="19">
+        <v>2</v>
+      </c>
+      <c r="P8" s="19">
+        <v>3</v>
+      </c>
+      <c r="Q8" s="19">
+        <v>4</v>
+      </c>
+      <c r="R8" s="19">
+        <v>5</v>
+      </c>
+      <c r="S8" s="19">
+        <v>6</v>
+      </c>
+      <c r="T8" s="19">
+        <v>7</v>
+      </c>
+      <c r="U8" s="19">
+        <v>8</v>
+      </c>
+      <c r="V8" s="19">
+        <v>9</v>
+      </c>
+      <c r="W8" s="19">
+        <v>10</v>
+      </c>
+      <c r="X8" s="19">
+        <v>11</v>
+      </c>
+      <c r="Y8" s="19">
+        <v>12</v>
+      </c>
+      <c r="Z8" s="19">
+        <v>13</v>
+      </c>
+      <c r="AA8" s="19">
+        <v>14</v>
+      </c>
+      <c r="AB8" s="19">
+        <v>15</v>
+      </c>
+      <c r="AC8" s="19">
+        <v>16</v>
+      </c>
+      <c r="AD8" s="19">
+        <v>17</v>
+      </c>
+      <c r="AE8" s="19">
+        <v>18</v>
+      </c>
+      <c r="AF8" s="19">
+        <v>19</v>
+      </c>
+      <c r="AG8" s="19">
+        <v>20</v>
+      </c>
+      <c r="AH8" s="19">
+        <v>21</v>
+      </c>
+      <c r="AI8" s="19">
+        <v>22</v>
+      </c>
+      <c r="AJ8" s="19">
+        <v>23</v>
+      </c>
+      <c r="AK8" s="19">
+        <v>24</v>
+      </c>
+      <c r="AL8" s="19">
+        <v>25</v>
+      </c>
+      <c r="AM8" s="19">
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="15">
         <v>42317</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="14" t="s">
         <v>8</v>
       </c>
       <c r="F9" s="8"/>
@@ -7038,13 +6808,13 @@
       <c r="A10">
         <v>2</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="15">
         <v>42338</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="14" t="s">
         <v>8</v>
       </c>
       <c r="I10" s="8"/>
@@ -7058,28 +6828,28 @@
       <c r="A11">
         <v>3</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="15">
         <v>42380</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="O11" s="17"/>
+      <c r="O11" s="16"/>
     </row>
     <row r="12" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>4</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="15">
         <v>42317</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F12" s="8"/>
@@ -7092,13 +6862,13 @@
       <c r="A13">
         <v>5</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="15">
         <v>42345</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="14" t="s">
         <v>25</v>
       </c>
       <c r="J13" s="8"/>
@@ -7114,13 +6884,13 @@
       <c r="A14">
         <v>6</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="15">
         <v>42380</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>40</v>
       </c>
       <c r="O14" s="7"/>
@@ -7132,13 +6902,13 @@
       <c r="A15">
         <v>7</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="15">
         <v>42401</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="14" t="s">
         <v>40</v>
       </c>
       <c r="P15" s="7"/>
@@ -7150,13 +6920,13 @@
       <c r="A16">
         <v>8</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="15">
         <v>42429</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="14" t="s">
         <v>25</v>
       </c>
       <c r="R16" s="7"/>
@@ -7174,10 +6944,10 @@
       <c r="B17" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="15">
         <v>42408</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="14" t="s">
         <v>25</v>
       </c>
       <c r="S17" s="7"/>
@@ -7195,13 +6965,13 @@
       <c r="A18">
         <v>10</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="15">
         <v>42394</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="14" t="s">
         <v>33</v>
       </c>
       <c r="Q18" s="7"/>
@@ -7223,13 +6993,13 @@
       <c r="A19">
         <v>11</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C19" s="15">
         <v>42492</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="14" t="s">
         <v>17</v>
       </c>
       <c r="AE19" s="7"/>
@@ -7238,13 +7008,13 @@
       <c r="A20">
         <v>12</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="16">
+      <c r="C20" s="15">
         <v>42499</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="14" t="s">
         <v>8</v>
       </c>
       <c r="AF20" s="7"/>
@@ -7257,113 +7027,113 @@
       <c r="A21">
         <v>13</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="16">
+      <c r="C21" s="15">
         <v>42534</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="14" t="s">
         <v>17</v>
       </c>
       <c r="AK21" s="7"/>
     </row>
     <row r="22" spans="1:39" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="10"/>
-      <c r="C22" s="16"/>
+      <c r="C22" s="15"/>
       <c r="D22" s="11"/>
     </row>
     <row r="23" spans="1:39" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="16">
+      <c r="C23" s="15">
         <v>42318</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="14" t="s">
         <v>6</v>
       </c>
       <c r="F23" s="8"/>
     </row>
     <row r="24" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="16">
+      <c r="C24" s="15">
         <v>42379</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="14" t="s">
         <v>6</v>
       </c>
       <c r="N24" s="8"/>
     </row>
     <row r="25" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="16">
+      <c r="C25" s="15">
         <v>42387</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="14" t="s">
         <v>6</v>
       </c>
       <c r="P25" s="7"/>
     </row>
     <row r="26" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="16">
+      <c r="C27" s="15">
         <v>42126</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D27" s="14" t="s">
         <v>6</v>
       </c>
       <c r="AD27" s="7"/>
     </row>
     <row r="28" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="16">
+      <c r="C28" s="15">
         <v>42133</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="14" t="s">
         <v>6</v>
       </c>
       <c r="AF28" s="7"/>
     </row>
     <row r="29" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="16">
+      <c r="C29" s="15">
         <v>42168</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="14" t="s">
         <v>6</v>
       </c>
       <c r="AJ29" s="7"/>
     </row>
     <row r="30" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="16">
+      <c r="C30" s="15">
         <v>42175</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D30" s="14" t="s">
         <v>6</v>
       </c>
       <c r="AK30" t="s">
@@ -7373,1142 +7143,1142 @@
     </row>
     <row r="31" spans="1:39" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="10"/>
-      <c r="C31" s="16"/>
+      <c r="C31" s="15"/>
       <c r="D31" s="11"/>
     </row>
     <row r="32" spans="1:39" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="16">
+      <c r="C32" s="15">
         <v>42325</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="14" t="s">
         <v>10</v>
       </c>
       <c r="G32" s="8"/>
     </row>
     <row r="33" spans="2:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="16">
+      <c r="C33" s="15">
         <v>42361</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="14" t="s">
         <v>13</v>
       </c>
       <c r="L33" s="8"/>
       <c r="M33" s="8"/>
     </row>
     <row r="34" spans="2:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="14"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="15"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:D4"/>
   </mergeCells>
   <conditionalFormatting sqref="G23:AM23 F32 H32:O32 F33:K34 N33:AM34 O10:AM10 P24:AM24 F24:H24 F25:O30 Q29:AI29 Q27:AC27 Q28:AE28 Q30:AK30 J34:Q34 Q25:AM26 AF27:AM27 AG28:AM28 AM30 AL29:AM29 F22:AM22 Q31:AM32 P11:AM11 P20:AE20 AK20:AM20 Y15:AM15 AB16:AM16 AE18:AM18 M9:AM9 M12:AM12 F15:N15 F11:N11 F20:N20 V13:AM13 W14:AM14 F18:P18 F16:R16">
-    <cfRule type="expression" dxfId="433" priority="601">
+    <cfRule type="expression" dxfId="417" priority="601">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="432" priority="603">
+    <cfRule type="expression" dxfId="416" priority="603">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="431" priority="604">
+    <cfRule type="expression" dxfId="415" priority="604">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="430" priority="605">
+    <cfRule type="expression" dxfId="414" priority="605">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="429" priority="606">
+    <cfRule type="expression" dxfId="413" priority="606">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="428" priority="607">
+    <cfRule type="expression" dxfId="412" priority="607">
       <formula>F$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="427" priority="611">
+    <cfRule type="expression" dxfId="411" priority="611">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="426" priority="612">
+    <cfRule type="expression" dxfId="410" priority="612">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35:AM35">
-    <cfRule type="expression" dxfId="425" priority="602">
+    <cfRule type="expression" dxfId="409" priority="602">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8:AM8">
-    <cfRule type="expression" dxfId="424" priority="608">
+    <cfRule type="expression" dxfId="408" priority="608">
       <formula>F$8=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="expression" dxfId="423" priority="577">
+    <cfRule type="expression" dxfId="407" priority="577">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="422" priority="578">
+    <cfRule type="expression" dxfId="406" priority="578">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="421" priority="579">
+    <cfRule type="expression" dxfId="405" priority="579">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="420" priority="580">
+    <cfRule type="expression" dxfId="404" priority="580">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="419" priority="581">
+    <cfRule type="expression" dxfId="403" priority="581">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="418" priority="582">
+    <cfRule type="expression" dxfId="402" priority="582">
       <formula>G$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="417" priority="583">
+    <cfRule type="expression" dxfId="401" priority="583">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="416" priority="584">
+    <cfRule type="expression" dxfId="400" priority="584">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="expression" dxfId="415" priority="569">
+    <cfRule type="expression" dxfId="399" priority="569">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="414" priority="570">
+    <cfRule type="expression" dxfId="398" priority="570">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="413" priority="571">
+    <cfRule type="expression" dxfId="397" priority="571">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="412" priority="572">
+    <cfRule type="expression" dxfId="396" priority="572">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="411" priority="573">
+    <cfRule type="expression" dxfId="395" priority="573">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="410" priority="574">
+    <cfRule type="expression" dxfId="394" priority="574">
       <formula>F$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="409" priority="575">
+    <cfRule type="expression" dxfId="393" priority="575">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="408" priority="576">
+    <cfRule type="expression" dxfId="392" priority="576">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24:M24">
-    <cfRule type="expression" dxfId="407" priority="529">
+    <cfRule type="expression" dxfId="391" priority="529">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="406" priority="530">
+    <cfRule type="expression" dxfId="390" priority="530">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="405" priority="531">
+    <cfRule type="expression" dxfId="389" priority="531">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="404" priority="532">
+    <cfRule type="expression" dxfId="388" priority="532">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="403" priority="533">
+    <cfRule type="expression" dxfId="387" priority="533">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="402" priority="534">
+    <cfRule type="expression" dxfId="386" priority="534">
       <formula>I$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="401" priority="535">
+    <cfRule type="expression" dxfId="385" priority="535">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="400" priority="536">
+    <cfRule type="expression" dxfId="384" priority="536">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O24">
-    <cfRule type="expression" dxfId="399" priority="521">
+    <cfRule type="expression" dxfId="383" priority="521">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="398" priority="522">
+    <cfRule type="expression" dxfId="382" priority="522">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="397" priority="523">
+    <cfRule type="expression" dxfId="381" priority="523">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="396" priority="524">
+    <cfRule type="expression" dxfId="380" priority="524">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="395" priority="525">
+    <cfRule type="expression" dxfId="379" priority="525">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="394" priority="526">
+    <cfRule type="expression" dxfId="378" priority="526">
       <formula>O$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="393" priority="527">
+    <cfRule type="expression" dxfId="377" priority="527">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="392" priority="528">
+    <cfRule type="expression" dxfId="376" priority="528">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14:J14 F13:I13">
-    <cfRule type="expression" dxfId="391" priority="505">
+    <cfRule type="expression" dxfId="375" priority="505">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="390" priority="506">
+    <cfRule type="expression" dxfId="374" priority="506">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="389" priority="507">
+    <cfRule type="expression" dxfId="373" priority="507">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="388" priority="508">
+    <cfRule type="expression" dxfId="372" priority="508">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="387" priority="509">
+    <cfRule type="expression" dxfId="371" priority="509">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="386" priority="510">
+    <cfRule type="expression" dxfId="370" priority="510">
       <formula>F$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="385" priority="511">
+    <cfRule type="expression" dxfId="369" priority="511">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="384" priority="512">
+    <cfRule type="expression" dxfId="368" priority="512">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14:N14">
-    <cfRule type="expression" dxfId="383" priority="497">
+    <cfRule type="expression" dxfId="367" priority="497">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="382" priority="498">
+    <cfRule type="expression" dxfId="366" priority="498">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="381" priority="499">
+    <cfRule type="expression" dxfId="365" priority="499">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="380" priority="500">
+    <cfRule type="expression" dxfId="364" priority="500">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="379" priority="501">
+    <cfRule type="expression" dxfId="363" priority="501">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="378" priority="502">
+    <cfRule type="expression" dxfId="362" priority="502">
       <formula>K$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="377" priority="503">
+    <cfRule type="expression" dxfId="361" priority="503">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="376" priority="504">
+    <cfRule type="expression" dxfId="360" priority="504">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F31:O31">
-    <cfRule type="expression" dxfId="375" priority="481">
+    <cfRule type="expression" dxfId="359" priority="481">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="374" priority="482">
+    <cfRule type="expression" dxfId="358" priority="482">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="373" priority="483">
+    <cfRule type="expression" dxfId="357" priority="483">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="372" priority="484">
+    <cfRule type="expression" dxfId="356" priority="484">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="371" priority="485">
+    <cfRule type="expression" dxfId="355" priority="485">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="370" priority="486">
+    <cfRule type="expression" dxfId="354" priority="486">
       <formula>F$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="369" priority="487">
+    <cfRule type="expression" dxfId="353" priority="487">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="368" priority="488">
+    <cfRule type="expression" dxfId="352" priority="488">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P26:P28">
-    <cfRule type="expression" dxfId="367" priority="473">
+    <cfRule type="expression" dxfId="351" priority="473">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="366" priority="474">
+    <cfRule type="expression" dxfId="350" priority="474">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="365" priority="475">
+    <cfRule type="expression" dxfId="349" priority="475">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="364" priority="476">
+    <cfRule type="expression" dxfId="348" priority="476">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="363" priority="477">
+    <cfRule type="expression" dxfId="347" priority="477">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="362" priority="478">
+    <cfRule type="expression" dxfId="346" priority="478">
       <formula>P$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="361" priority="479">
+    <cfRule type="expression" dxfId="345" priority="479">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="360" priority="480">
+    <cfRule type="expression" dxfId="344" priority="480">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P29:P32">
-    <cfRule type="expression" dxfId="359" priority="465">
+    <cfRule type="expression" dxfId="343" priority="465">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="358" priority="466">
+    <cfRule type="expression" dxfId="342" priority="466">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="357" priority="467">
+    <cfRule type="expression" dxfId="341" priority="467">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="356" priority="468">
+    <cfRule type="expression" dxfId="340" priority="468">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="355" priority="469">
+    <cfRule type="expression" dxfId="339" priority="469">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="354" priority="470">
+    <cfRule type="expression" dxfId="338" priority="470">
       <formula>P$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="353" priority="471">
+    <cfRule type="expression" dxfId="337" priority="471">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="352" priority="472">
+    <cfRule type="expression" dxfId="336" priority="472">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE27">
-    <cfRule type="expression" dxfId="351" priority="457">
+    <cfRule type="expression" dxfId="335" priority="457">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="350" priority="458">
+    <cfRule type="expression" dxfId="334" priority="458">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="349" priority="459">
+    <cfRule type="expression" dxfId="333" priority="459">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="348" priority="460">
+    <cfRule type="expression" dxfId="332" priority="460">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="347" priority="461">
+    <cfRule type="expression" dxfId="331" priority="461">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="346" priority="462">
+    <cfRule type="expression" dxfId="330" priority="462">
       <formula>AE$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="345" priority="463">
+    <cfRule type="expression" dxfId="329" priority="463">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="344" priority="464">
+    <cfRule type="expression" dxfId="328" priority="464">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK29">
-    <cfRule type="expression" dxfId="343" priority="449">
+    <cfRule type="expression" dxfId="327" priority="449">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="342" priority="450">
+    <cfRule type="expression" dxfId="326" priority="450">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="341" priority="451">
+    <cfRule type="expression" dxfId="325" priority="451">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="340" priority="452">
+    <cfRule type="expression" dxfId="324" priority="452">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="339" priority="453">
+    <cfRule type="expression" dxfId="323" priority="453">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="338" priority="454">
+    <cfRule type="expression" dxfId="322" priority="454">
       <formula>AK$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="337" priority="455">
+    <cfRule type="expression" dxfId="321" priority="455">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="336" priority="456">
+    <cfRule type="expression" dxfId="320" priority="456">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q13:S13">
-    <cfRule type="expression" dxfId="335" priority="441">
+    <cfRule type="expression" dxfId="319" priority="441">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="334" priority="442">
+    <cfRule type="expression" dxfId="318" priority="442">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="333" priority="443">
+    <cfRule type="expression" dxfId="317" priority="443">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="332" priority="444">
+    <cfRule type="expression" dxfId="316" priority="444">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="331" priority="445">
+    <cfRule type="expression" dxfId="315" priority="445">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="330" priority="446">
+    <cfRule type="expression" dxfId="314" priority="446">
       <formula>Q$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="329" priority="447">
+    <cfRule type="expression" dxfId="313" priority="447">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="328" priority="448">
+    <cfRule type="expression" dxfId="312" priority="448">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T14">
-    <cfRule type="expression" dxfId="327" priority="433">
+    <cfRule type="expression" dxfId="311" priority="433">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="326" priority="434">
+    <cfRule type="expression" dxfId="310" priority="434">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="325" priority="435">
+    <cfRule type="expression" dxfId="309" priority="435">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="324" priority="436">
+    <cfRule type="expression" dxfId="308" priority="436">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="323" priority="437">
+    <cfRule type="expression" dxfId="307" priority="437">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="322" priority="438">
+    <cfRule type="expression" dxfId="306" priority="438">
       <formula>T$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="321" priority="439">
+    <cfRule type="expression" dxfId="305" priority="439">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="320" priority="440">
+    <cfRule type="expression" dxfId="304" priority="440">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9">
-    <cfRule type="expression" dxfId="319" priority="425">
+    <cfRule type="expression" dxfId="303" priority="425">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="318" priority="426">
+    <cfRule type="expression" dxfId="302" priority="426">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="317" priority="427">
+    <cfRule type="expression" dxfId="301" priority="427">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="316" priority="428">
+    <cfRule type="expression" dxfId="300" priority="428">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="315" priority="429">
+    <cfRule type="expression" dxfId="299" priority="429">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="314" priority="430">
+    <cfRule type="expression" dxfId="298" priority="430">
       <formula>L$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="313" priority="431">
+    <cfRule type="expression" dxfId="297" priority="431">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="312" priority="432">
+    <cfRule type="expression" dxfId="296" priority="432">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O15 O20">
-    <cfRule type="expression" dxfId="311" priority="393">
+    <cfRule type="expression" dxfId="295" priority="393">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="310" priority="394">
+    <cfRule type="expression" dxfId="294" priority="394">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="309" priority="395">
+    <cfRule type="expression" dxfId="293" priority="395">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="308" priority="396">
+    <cfRule type="expression" dxfId="292" priority="396">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="307" priority="397">
+    <cfRule type="expression" dxfId="291" priority="397">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="306" priority="398">
+    <cfRule type="expression" dxfId="290" priority="398">
       <formula>O$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="305" priority="399">
+    <cfRule type="expression" dxfId="289" priority="399">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="304" priority="400">
+    <cfRule type="expression" dxfId="288" priority="400">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S14">
-    <cfRule type="expression" dxfId="303" priority="353">
+    <cfRule type="expression" dxfId="287" priority="353">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="302" priority="354">
+    <cfRule type="expression" dxfId="286" priority="354">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="301" priority="355">
+    <cfRule type="expression" dxfId="285" priority="355">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="300" priority="356">
+    <cfRule type="expression" dxfId="284" priority="356">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="299" priority="357">
+    <cfRule type="expression" dxfId="283" priority="357">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="298" priority="358">
+    <cfRule type="expression" dxfId="282" priority="358">
       <formula>S$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="297" priority="359">
+    <cfRule type="expression" dxfId="281" priority="359">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="296" priority="360">
+    <cfRule type="expression" dxfId="280" priority="360">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="expression" dxfId="295" priority="337">
+    <cfRule type="expression" dxfId="279" priority="337">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="294" priority="338">
+    <cfRule type="expression" dxfId="278" priority="338">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="293" priority="339">
+    <cfRule type="expression" dxfId="277" priority="339">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="292" priority="340">
+    <cfRule type="expression" dxfId="276" priority="340">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="291" priority="341">
+    <cfRule type="expression" dxfId="275" priority="341">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="290" priority="342">
+    <cfRule type="expression" dxfId="274" priority="342">
       <formula>H$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="289" priority="343">
+    <cfRule type="expression" dxfId="273" priority="343">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="288" priority="344">
+    <cfRule type="expression" dxfId="272" priority="344">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12:L12">
-    <cfRule type="expression" dxfId="287" priority="329">
+    <cfRule type="expression" dxfId="271" priority="329">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="286" priority="330">
+    <cfRule type="expression" dxfId="270" priority="330">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="285" priority="331">
+    <cfRule type="expression" dxfId="269" priority="331">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="284" priority="332">
+    <cfRule type="expression" dxfId="268" priority="332">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="283" priority="333">
+    <cfRule type="expression" dxfId="267" priority="333">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="282" priority="334">
+    <cfRule type="expression" dxfId="266" priority="334">
       <formula>K$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="281" priority="335">
+    <cfRule type="expression" dxfId="265" priority="335">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="280" priority="336">
+    <cfRule type="expression" dxfId="264" priority="336">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U16">
-    <cfRule type="expression" dxfId="279" priority="369">
+    <cfRule type="expression" dxfId="263" priority="369">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="278" priority="370">
+    <cfRule type="expression" dxfId="262" priority="370">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="277" priority="371">
+    <cfRule type="expression" dxfId="261" priority="371">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="276" priority="372">
+    <cfRule type="expression" dxfId="260" priority="372">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="275" priority="373">
+    <cfRule type="expression" dxfId="259" priority="373">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="274" priority="374">
+    <cfRule type="expression" dxfId="258" priority="374">
       <formula>U$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="273" priority="375">
+    <cfRule type="expression" dxfId="257" priority="375">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="272" priority="376">
+    <cfRule type="expression" dxfId="256" priority="376">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19:AD19 AF19:AM19">
-    <cfRule type="expression" dxfId="271" priority="313">
+    <cfRule type="expression" dxfId="255" priority="313">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="270" priority="314">
+    <cfRule type="expression" dxfId="254" priority="314">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="269" priority="315">
+    <cfRule type="expression" dxfId="253" priority="315">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="268" priority="316">
+    <cfRule type="expression" dxfId="252" priority="316">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="267" priority="317">
+    <cfRule type="expression" dxfId="251" priority="317">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="266" priority="318">
+    <cfRule type="expression" dxfId="250" priority="318">
       <formula>F$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="265" priority="319">
+    <cfRule type="expression" dxfId="249" priority="319">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="264" priority="320">
+    <cfRule type="expression" dxfId="248" priority="320">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21:AJ21 AL21:AM21">
-    <cfRule type="expression" dxfId="263" priority="305">
+    <cfRule type="expression" dxfId="247" priority="305">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="262" priority="306">
+    <cfRule type="expression" dxfId="246" priority="306">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="261" priority="307">
+    <cfRule type="expression" dxfId="245" priority="307">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="260" priority="308">
+    <cfRule type="expression" dxfId="244" priority="308">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="259" priority="309">
+    <cfRule type="expression" dxfId="243" priority="309">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="258" priority="310">
+    <cfRule type="expression" dxfId="242" priority="310">
       <formula>F$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="257" priority="311">
+    <cfRule type="expression" dxfId="241" priority="311">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="256" priority="312">
+    <cfRule type="expression" dxfId="240" priority="312">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q14">
-    <cfRule type="expression" dxfId="255" priority="297">
+    <cfRule type="expression" dxfId="239" priority="297">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="254" priority="298">
+    <cfRule type="expression" dxfId="238" priority="298">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="253" priority="299">
+    <cfRule type="expression" dxfId="237" priority="299">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="252" priority="300">
+    <cfRule type="expression" dxfId="236" priority="300">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="251" priority="301">
+    <cfRule type="expression" dxfId="235" priority="301">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="250" priority="302">
+    <cfRule type="expression" dxfId="234" priority="302">
       <formula>Q$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="249" priority="303">
+    <cfRule type="expression" dxfId="233" priority="303">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="248" priority="304">
+    <cfRule type="expression" dxfId="232" priority="304">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R14">
-    <cfRule type="expression" dxfId="247" priority="289">
+    <cfRule type="expression" dxfId="231" priority="289">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="246" priority="290">
+    <cfRule type="expression" dxfId="230" priority="290">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="245" priority="291">
+    <cfRule type="expression" dxfId="229" priority="291">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="244" priority="292">
+    <cfRule type="expression" dxfId="228" priority="292">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="243" priority="293">
+    <cfRule type="expression" dxfId="227" priority="293">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="242" priority="294">
+    <cfRule type="expression" dxfId="226" priority="294">
       <formula>R$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="241" priority="295">
+    <cfRule type="expression" dxfId="225" priority="295">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="240" priority="296">
+    <cfRule type="expression" dxfId="224" priority="296">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S15">
-    <cfRule type="expression" dxfId="239" priority="281">
+    <cfRule type="expression" dxfId="223" priority="281">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="238" priority="282">
+    <cfRule type="expression" dxfId="222" priority="282">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="237" priority="283">
+    <cfRule type="expression" dxfId="221" priority="283">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="236" priority="284">
+    <cfRule type="expression" dxfId="220" priority="284">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="235" priority="285">
+    <cfRule type="expression" dxfId="219" priority="285">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="234" priority="286">
+    <cfRule type="expression" dxfId="218" priority="286">
       <formula>S$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="233" priority="287">
+    <cfRule type="expression" dxfId="217" priority="287">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="232" priority="288">
+    <cfRule type="expression" dxfId="216" priority="288">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T15">
-    <cfRule type="expression" dxfId="231" priority="273">
+    <cfRule type="expression" dxfId="215" priority="273">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="230" priority="274">
+    <cfRule type="expression" dxfId="214" priority="274">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="229" priority="275">
+    <cfRule type="expression" dxfId="213" priority="275">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="228" priority="276">
+    <cfRule type="expression" dxfId="212" priority="276">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="227" priority="277">
+    <cfRule type="expression" dxfId="211" priority="277">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="226" priority="278">
+    <cfRule type="expression" dxfId="210" priority="278">
       <formula>T$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="225" priority="279">
+    <cfRule type="expression" dxfId="209" priority="279">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="224" priority="280">
+    <cfRule type="expression" dxfId="208" priority="280">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V16">
-    <cfRule type="expression" dxfId="223" priority="265">
+    <cfRule type="expression" dxfId="207" priority="265">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="222" priority="266">
+    <cfRule type="expression" dxfId="206" priority="266">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="221" priority="267">
+    <cfRule type="expression" dxfId="205" priority="267">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="220" priority="268">
+    <cfRule type="expression" dxfId="204" priority="268">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="219" priority="269">
+    <cfRule type="expression" dxfId="203" priority="269">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="218" priority="270">
+    <cfRule type="expression" dxfId="202" priority="270">
       <formula>V$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="217" priority="271">
+    <cfRule type="expression" dxfId="201" priority="271">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="216" priority="272">
+    <cfRule type="expression" dxfId="200" priority="272">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W16">
-    <cfRule type="expression" dxfId="215" priority="257">
+    <cfRule type="expression" dxfId="199" priority="257">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="214" priority="258">
+    <cfRule type="expression" dxfId="198" priority="258">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="213" priority="259">
+    <cfRule type="expression" dxfId="197" priority="259">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="212" priority="260">
+    <cfRule type="expression" dxfId="196" priority="260">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="211" priority="261">
+    <cfRule type="expression" dxfId="195" priority="261">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="210" priority="262">
+    <cfRule type="expression" dxfId="194" priority="262">
       <formula>W$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="209" priority="263">
+    <cfRule type="expression" dxfId="193" priority="263">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="208" priority="264">
+    <cfRule type="expression" dxfId="192" priority="264">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U15">
-    <cfRule type="expression" dxfId="207" priority="249">
+    <cfRule type="expression" dxfId="191" priority="249">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="206" priority="250">
+    <cfRule type="expression" dxfId="190" priority="250">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="205" priority="251">
+    <cfRule type="expression" dxfId="189" priority="251">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="204" priority="252">
+    <cfRule type="expression" dxfId="188" priority="252">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="203" priority="253">
+    <cfRule type="expression" dxfId="187" priority="253">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="202" priority="254">
+    <cfRule type="expression" dxfId="186" priority="254">
       <formula>U$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="201" priority="255">
+    <cfRule type="expression" dxfId="185" priority="255">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="200" priority="256">
+    <cfRule type="expression" dxfId="184" priority="256">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T16">
-    <cfRule type="expression" dxfId="199" priority="177">
+    <cfRule type="expression" dxfId="183" priority="177">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="198" priority="178">
+    <cfRule type="expression" dxfId="182" priority="178">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="197" priority="179">
+    <cfRule type="expression" dxfId="181" priority="179">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="196" priority="180">
+    <cfRule type="expression" dxfId="180" priority="180">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="195" priority="181">
+    <cfRule type="expression" dxfId="179" priority="181">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="194" priority="182">
+    <cfRule type="expression" dxfId="178" priority="182">
       <formula>T$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="193" priority="183">
+    <cfRule type="expression" dxfId="177" priority="183">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="192" priority="184">
+    <cfRule type="expression" dxfId="176" priority="184">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N13">
-    <cfRule type="expression" dxfId="191" priority="209">
+    <cfRule type="expression" dxfId="175" priority="209">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="190" priority="210">
+    <cfRule type="expression" dxfId="174" priority="210">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="189" priority="211">
+    <cfRule type="expression" dxfId="173" priority="211">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="188" priority="212">
+    <cfRule type="expression" dxfId="172" priority="212">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="187" priority="213">
+    <cfRule type="expression" dxfId="171" priority="213">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="186" priority="214">
+    <cfRule type="expression" dxfId="170" priority="214">
       <formula>N$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="185" priority="215">
+    <cfRule type="expression" dxfId="169" priority="215">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="184" priority="216">
+    <cfRule type="expression" dxfId="168" priority="216">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X15">
-    <cfRule type="expression" dxfId="183" priority="161">
+    <cfRule type="expression" dxfId="167" priority="161">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="182" priority="162">
+    <cfRule type="expression" dxfId="166" priority="162">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="181" priority="163">
+    <cfRule type="expression" dxfId="165" priority="163">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="180" priority="164">
+    <cfRule type="expression" dxfId="164" priority="164">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="179" priority="165">
+    <cfRule type="expression" dxfId="163" priority="165">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="178" priority="166">
+    <cfRule type="expression" dxfId="162" priority="166">
       <formula>X$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="177" priority="167">
+    <cfRule type="expression" dxfId="161" priority="167">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="176" priority="168">
+    <cfRule type="expression" dxfId="160" priority="168">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R15">
-    <cfRule type="expression" dxfId="167" priority="185">
+    <cfRule type="expression" dxfId="159" priority="185">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="166" priority="186">
+    <cfRule type="expression" dxfId="158" priority="186">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="165" priority="187">
+    <cfRule type="expression" dxfId="157" priority="187">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="164" priority="188">
+    <cfRule type="expression" dxfId="156" priority="188">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="163" priority="189">
+    <cfRule type="expression" dxfId="155" priority="189">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="162" priority="190">
+    <cfRule type="expression" dxfId="154" priority="190">
       <formula>R$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="161" priority="191">
+    <cfRule type="expression" dxfId="153" priority="191">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="160" priority="192">
+    <cfRule type="expression" dxfId="152" priority="192">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA16">
-    <cfRule type="expression" dxfId="159" priority="169">
+    <cfRule type="expression" dxfId="151" priority="169">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="158" priority="170">
+    <cfRule type="expression" dxfId="150" priority="170">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="157" priority="171">
+    <cfRule type="expression" dxfId="149" priority="171">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="156" priority="172">
+    <cfRule type="expression" dxfId="148" priority="172">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="155" priority="173">
+    <cfRule type="expression" dxfId="147" priority="173">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="154" priority="174">
+    <cfRule type="expression" dxfId="146" priority="174">
       <formula>AA$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="153" priority="175">
+    <cfRule type="expression" dxfId="145" priority="175">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="152" priority="176">
+    <cfRule type="expression" dxfId="144" priority="176">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U13">
-    <cfRule type="expression" dxfId="151" priority="145">
+    <cfRule type="expression" dxfId="143" priority="145">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="150" priority="146">
+    <cfRule type="expression" dxfId="142" priority="146">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="149" priority="147">
+    <cfRule type="expression" dxfId="141" priority="147">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="148" priority="148">
+    <cfRule type="expression" dxfId="140" priority="148">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="147" priority="149">
+    <cfRule type="expression" dxfId="139" priority="149">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="146" priority="150">
+    <cfRule type="expression" dxfId="138" priority="150">
       <formula>U$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="145" priority="151">
+    <cfRule type="expression" dxfId="137" priority="151">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="144" priority="152">
+    <cfRule type="expression" dxfId="136" priority="152">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P13">
-    <cfRule type="expression" dxfId="143" priority="137">
+    <cfRule type="expression" dxfId="135" priority="137">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="142" priority="138">
+    <cfRule type="expression" dxfId="134" priority="138">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="141" priority="139">
+    <cfRule type="expression" dxfId="133" priority="139">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="140" priority="140">
+    <cfRule type="expression" dxfId="132" priority="140">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="139" priority="141">
+    <cfRule type="expression" dxfId="131" priority="141">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="138" priority="142">
+    <cfRule type="expression" dxfId="130" priority="142">
       <formula>P$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="137" priority="143">
+    <cfRule type="expression" dxfId="129" priority="143">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="136" priority="144">
+    <cfRule type="expression" dxfId="128" priority="144">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17">
-    <cfRule type="expression" dxfId="135" priority="129">
+    <cfRule type="expression" dxfId="127" priority="129">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="134" priority="130">
+    <cfRule type="expression" dxfId="126" priority="130">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="133" priority="131">
+    <cfRule type="expression" dxfId="125" priority="131">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="132" priority="132">
+    <cfRule type="expression" dxfId="124" priority="132">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="131" priority="133">
+    <cfRule type="expression" dxfId="123" priority="133">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="130" priority="134">
+    <cfRule type="expression" dxfId="122" priority="134">
       <formula>G$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="129" priority="135">
+    <cfRule type="expression" dxfId="121" priority="135">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="128" priority="136">
+    <cfRule type="expression" dxfId="120" priority="136">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17">
-    <cfRule type="expression" dxfId="127" priority="121">
+    <cfRule type="expression" dxfId="119" priority="121">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="126" priority="122">
+    <cfRule type="expression" dxfId="118" priority="122">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="123">
+    <cfRule type="expression" dxfId="117" priority="123">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="124">
+    <cfRule type="expression" dxfId="116" priority="124">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="125">
+    <cfRule type="expression" dxfId="115" priority="125">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="126">
+    <cfRule type="expression" dxfId="114" priority="126">
       <formula>I$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="121" priority="127">
+    <cfRule type="expression" dxfId="113" priority="127">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="120" priority="128">
+    <cfRule type="expression" dxfId="112" priority="128">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17">
-    <cfRule type="expression" dxfId="119" priority="113">
+    <cfRule type="expression" dxfId="111" priority="113">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="114">
+    <cfRule type="expression" dxfId="110" priority="114">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="115">
+    <cfRule type="expression" dxfId="109" priority="115">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="116">
+    <cfRule type="expression" dxfId="108" priority="116">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="117">
+    <cfRule type="expression" dxfId="107" priority="117">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="118">
+    <cfRule type="expression" dxfId="106" priority="118">
       <formula>K$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="119">
+    <cfRule type="expression" dxfId="105" priority="119">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="120">
+    <cfRule type="expression" dxfId="104" priority="120">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M17">
-    <cfRule type="expression" dxfId="111" priority="105">
+    <cfRule type="expression" dxfId="103" priority="105">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="106">
+    <cfRule type="expression" dxfId="102" priority="106">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="107">
+    <cfRule type="expression" dxfId="101" priority="107">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="108">
+    <cfRule type="expression" dxfId="100" priority="108">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="109">
+    <cfRule type="expression" dxfId="99" priority="109">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="110">
+    <cfRule type="expression" dxfId="98" priority="110">
       <formula>M$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="111">
+    <cfRule type="expression" dxfId="97" priority="111">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="112">
+    <cfRule type="expression" dxfId="96" priority="112">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O17">
-    <cfRule type="expression" dxfId="103" priority="97">
+    <cfRule type="expression" dxfId="95" priority="97">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="98">
+    <cfRule type="expression" dxfId="94" priority="98">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="99">
+    <cfRule type="expression" dxfId="93" priority="99">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="100">
+    <cfRule type="expression" dxfId="92" priority="100">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="101">
+    <cfRule type="expression" dxfId="91" priority="101">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="102">
+    <cfRule type="expression" dxfId="90" priority="102">
       <formula>O$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="103">
+    <cfRule type="expression" dxfId="89" priority="103">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="104">
+    <cfRule type="expression" dxfId="88" priority="104">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17">
-    <cfRule type="expression" dxfId="95" priority="89">
+    <cfRule type="expression" dxfId="87" priority="89">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="90">
+    <cfRule type="expression" dxfId="86" priority="90">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="91">
+    <cfRule type="expression" dxfId="85" priority="91">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="92">
+    <cfRule type="expression" dxfId="84" priority="92">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="93">
+    <cfRule type="expression" dxfId="83" priority="93">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="94">
+    <cfRule type="expression" dxfId="82" priority="94">
       <formula>Q$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="95">
+    <cfRule type="expression" dxfId="81" priority="95">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="96">
+    <cfRule type="expression" dxfId="80" priority="96">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>